<commit_message>
M3 Cord Production System #985 - Implements Solution Export #3 - Update App build 1342
</commit_message>
<xml_diff>
--- a/05.Controls/M3.Cord.Controls/Resources/Excels/AX_09PV3_8335.xlsx
+++ b/05.Controls/M3.Cord.Controls/Resources/Excels/AX_09PV3_8335.xlsx
@@ -2487,7 +2487,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="313">
+  <cellXfs count="311">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
@@ -3028,9 +3028,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="54" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="32" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -3199,6 +3196,114 @@
     <xf numFmtId="2" fontId="46" fillId="4" borderId="47" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="47" fillId="4" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="4" borderId="10" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="47" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="30" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="47" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="47" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="30" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="4" borderId="47" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="47" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="47" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="4" borderId="30" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="49" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="49" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="42" fillId="2" borderId="53" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="42" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="42" fillId="0" borderId="4" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="42" fillId="2" borderId="18" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="42" fillId="2" borderId="19" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="42" fillId="2" borderId="25" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="42" fillId="2" borderId="26" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="2" borderId="21" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="2" borderId="22" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="41" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="52" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="44" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="37" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3232,12 +3337,6 @@
     <xf numFmtId="0" fontId="38" fillId="0" borderId="50" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="69" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3255,111 +3354,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="41" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="52" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="44" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="42" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="42" fillId="0" borderId="4" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="42" fillId="2" borderId="18" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="42" fillId="2" borderId="19" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="42" fillId="2" borderId="25" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="42" fillId="2" borderId="26" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="2" borderId="21" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="2" borderId="22" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="47" fillId="4" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="4" borderId="10" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="47" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="30" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="47" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="47" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="30" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="4" borderId="47" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="47" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="47" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="4" borderId="30" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="49" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="49" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="42" fillId="2" borderId="53" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -3402,7 +3396,7 @@
         <xdr:cNvPr id="4" name="Oval 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{85863F61-999D-4DCE-B07B-E9EA35273305}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{85863F61-999D-4DCE-B07B-E9EA35273305}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3451,7 +3445,7 @@
         <xdr:cNvPr id="5" name="Oval 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5E1BC519-940B-4402-871B-35C4EFE4B33D}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5E1BC519-940B-4402-871B-35C4EFE4B33D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3500,7 +3494,7 @@
         <xdr:cNvPr id="6" name="Oval 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{15C2E9E0-E060-482F-B280-F2F04D9F6A69}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15C2E9E0-E060-482F-B280-F2F04D9F6A69}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3549,7 +3543,7 @@
         <xdr:cNvPr id="7" name="Oval 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C0A0A530-34CB-429D-ABF4-B485669B93A9}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0A0A530-34CB-429D-ABF4-B485669B93A9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3598,7 +3592,7 @@
         <xdr:cNvPr id="8" name="Picture 26" descr="TORAY_blue_set(B).png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{855D66E7-6BDE-42DE-A912-36CF16FFBC27}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{855D66E7-6BDE-42DE-A912-36CF16FFBC27}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3610,7 +3604,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -3633,14 +3627,14 @@
         </a:ln>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -3672,7 +3666,7 @@
         <xdr:cNvPr id="9" name="Picture 26" descr="TORAY_blue_set(B).png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{67DB5453-CD40-4750-9897-6418948331BD}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{67DB5453-CD40-4750-9897-6418948331BD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3684,7 +3678,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -3707,14 +3701,14 @@
         </a:ln>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -3746,7 +3740,7 @@
         <xdr:cNvPr id="10" name="Oval 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{ECDCD752-11A1-4E5E-B8E0-53BAC292349C}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ECDCD752-11A1-4E5E-B8E0-53BAC292349C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3795,7 +3789,7 @@
         <xdr:cNvPr id="11" name="Oval 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BF2503BA-BFCC-42AF-A82F-67486839EC6F}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF2503BA-BFCC-42AF-A82F-67486839EC6F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3844,7 +3838,7 @@
         <xdr:cNvPr id="12" name="Oval 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A3CC89CB-F622-4E82-A982-5198E092825A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3CC89CB-F622-4E82-A982-5198E092825A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3893,7 +3887,7 @@
         <xdr:cNvPr id="13" name="Oval 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F473927F-C703-4A34-8248-D504340A516F}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F473927F-C703-4A34-8248-D504340A516F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4216,7 +4210,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4227,719 +4221,719 @@
   <dimension ref="A1:S82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G55" sqref="G55"/>
+      <selection activeCell="B4" sqref="B4:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="19.8"/>
   <cols>
-    <col min="1" max="2" width="10" style="238" customWidth="1"/>
-    <col min="3" max="3" width="18" style="238" customWidth="1"/>
-    <col min="4" max="4" width="16" style="238" customWidth="1"/>
-    <col min="5" max="6" width="8.625" style="238" customWidth="1"/>
-    <col min="7" max="7" width="12.875" style="238" customWidth="1"/>
-    <col min="8" max="8" width="14.75" style="238" customWidth="1"/>
-    <col min="9" max="9" width="14.125" style="238" customWidth="1"/>
-    <col min="10" max="10" width="14.75" style="238" customWidth="1"/>
-    <col min="11" max="11" width="9.125" style="238"/>
-    <col min="12" max="12" width="17" style="238" hidden="1" customWidth="1"/>
+    <col min="1" max="2" width="10" style="237" customWidth="1"/>
+    <col min="3" max="3" width="18" style="237" customWidth="1"/>
+    <col min="4" max="4" width="16" style="237" customWidth="1"/>
+    <col min="5" max="6" width="8.625" style="237" customWidth="1"/>
+    <col min="7" max="7" width="12.875" style="237" customWidth="1"/>
+    <col min="8" max="8" width="14.75" style="237" customWidth="1"/>
+    <col min="9" max="9" width="14.125" style="237" customWidth="1"/>
+    <col min="10" max="10" width="14.75" style="237" customWidth="1"/>
+    <col min="11" max="11" width="9.125" style="237"/>
+    <col min="12" max="12" width="17" style="237" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="17.25" style="6" hidden="1" customWidth="1"/>
     <col min="14" max="18" width="0" style="6" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="17.75" style="238" hidden="1" customWidth="1"/>
-    <col min="20" max="22" width="0" style="238" hidden="1" customWidth="1"/>
-    <col min="23" max="256" width="9.125" style="238"/>
-    <col min="257" max="258" width="10" style="238" customWidth="1"/>
-    <col min="259" max="259" width="18" style="238" customWidth="1"/>
-    <col min="260" max="260" width="16" style="238" customWidth="1"/>
-    <col min="261" max="262" width="8.625" style="238" customWidth="1"/>
-    <col min="263" max="263" width="12.875" style="238" customWidth="1"/>
-    <col min="264" max="264" width="14.75" style="238" customWidth="1"/>
-    <col min="265" max="265" width="14.125" style="238" customWidth="1"/>
-    <col min="266" max="266" width="14.75" style="238" customWidth="1"/>
-    <col min="267" max="267" width="9.125" style="238"/>
-    <col min="268" max="278" width="0" style="238" hidden="1" customWidth="1"/>
-    <col min="279" max="512" width="9.125" style="238"/>
-    <col min="513" max="514" width="10" style="238" customWidth="1"/>
-    <col min="515" max="515" width="18" style="238" customWidth="1"/>
-    <col min="516" max="516" width="16" style="238" customWidth="1"/>
-    <col min="517" max="518" width="8.625" style="238" customWidth="1"/>
-    <col min="519" max="519" width="12.875" style="238" customWidth="1"/>
-    <col min="520" max="520" width="14.75" style="238" customWidth="1"/>
-    <col min="521" max="521" width="14.125" style="238" customWidth="1"/>
-    <col min="522" max="522" width="14.75" style="238" customWidth="1"/>
-    <col min="523" max="523" width="9.125" style="238"/>
-    <col min="524" max="534" width="0" style="238" hidden="1" customWidth="1"/>
-    <col min="535" max="768" width="9.125" style="238"/>
-    <col min="769" max="770" width="10" style="238" customWidth="1"/>
-    <col min="771" max="771" width="18" style="238" customWidth="1"/>
-    <col min="772" max="772" width="16" style="238" customWidth="1"/>
-    <col min="773" max="774" width="8.625" style="238" customWidth="1"/>
-    <col min="775" max="775" width="12.875" style="238" customWidth="1"/>
-    <col min="776" max="776" width="14.75" style="238" customWidth="1"/>
-    <col min="777" max="777" width="14.125" style="238" customWidth="1"/>
-    <col min="778" max="778" width="14.75" style="238" customWidth="1"/>
-    <col min="779" max="779" width="9.125" style="238"/>
-    <col min="780" max="790" width="0" style="238" hidden="1" customWidth="1"/>
-    <col min="791" max="1024" width="9.125" style="238"/>
-    <col min="1025" max="1026" width="10" style="238" customWidth="1"/>
-    <col min="1027" max="1027" width="18" style="238" customWidth="1"/>
-    <col min="1028" max="1028" width="16" style="238" customWidth="1"/>
-    <col min="1029" max="1030" width="8.625" style="238" customWidth="1"/>
-    <col min="1031" max="1031" width="12.875" style="238" customWidth="1"/>
-    <col min="1032" max="1032" width="14.75" style="238" customWidth="1"/>
-    <col min="1033" max="1033" width="14.125" style="238" customWidth="1"/>
-    <col min="1034" max="1034" width="14.75" style="238" customWidth="1"/>
-    <col min="1035" max="1035" width="9.125" style="238"/>
-    <col min="1036" max="1046" width="0" style="238" hidden="1" customWidth="1"/>
-    <col min="1047" max="1280" width="9.125" style="238"/>
-    <col min="1281" max="1282" width="10" style="238" customWidth="1"/>
-    <col min="1283" max="1283" width="18" style="238" customWidth="1"/>
-    <col min="1284" max="1284" width="16" style="238" customWidth="1"/>
-    <col min="1285" max="1286" width="8.625" style="238" customWidth="1"/>
-    <col min="1287" max="1287" width="12.875" style="238" customWidth="1"/>
-    <col min="1288" max="1288" width="14.75" style="238" customWidth="1"/>
-    <col min="1289" max="1289" width="14.125" style="238" customWidth="1"/>
-    <col min="1290" max="1290" width="14.75" style="238" customWidth="1"/>
-    <col min="1291" max="1291" width="9.125" style="238"/>
-    <col min="1292" max="1302" width="0" style="238" hidden="1" customWidth="1"/>
-    <col min="1303" max="1536" width="9.125" style="238"/>
-    <col min="1537" max="1538" width="10" style="238" customWidth="1"/>
-    <col min="1539" max="1539" width="18" style="238" customWidth="1"/>
-    <col min="1540" max="1540" width="16" style="238" customWidth="1"/>
-    <col min="1541" max="1542" width="8.625" style="238" customWidth="1"/>
-    <col min="1543" max="1543" width="12.875" style="238" customWidth="1"/>
-    <col min="1544" max="1544" width="14.75" style="238" customWidth="1"/>
-    <col min="1545" max="1545" width="14.125" style="238" customWidth="1"/>
-    <col min="1546" max="1546" width="14.75" style="238" customWidth="1"/>
-    <col min="1547" max="1547" width="9.125" style="238"/>
-    <col min="1548" max="1558" width="0" style="238" hidden="1" customWidth="1"/>
-    <col min="1559" max="1792" width="9.125" style="238"/>
-    <col min="1793" max="1794" width="10" style="238" customWidth="1"/>
-    <col min="1795" max="1795" width="18" style="238" customWidth="1"/>
-    <col min="1796" max="1796" width="16" style="238" customWidth="1"/>
-    <col min="1797" max="1798" width="8.625" style="238" customWidth="1"/>
-    <col min="1799" max="1799" width="12.875" style="238" customWidth="1"/>
-    <col min="1800" max="1800" width="14.75" style="238" customWidth="1"/>
-    <col min="1801" max="1801" width="14.125" style="238" customWidth="1"/>
-    <col min="1802" max="1802" width="14.75" style="238" customWidth="1"/>
-    <col min="1803" max="1803" width="9.125" style="238"/>
-    <col min="1804" max="1814" width="0" style="238" hidden="1" customWidth="1"/>
-    <col min="1815" max="2048" width="9.125" style="238"/>
-    <col min="2049" max="2050" width="10" style="238" customWidth="1"/>
-    <col min="2051" max="2051" width="18" style="238" customWidth="1"/>
-    <col min="2052" max="2052" width="16" style="238" customWidth="1"/>
-    <col min="2053" max="2054" width="8.625" style="238" customWidth="1"/>
-    <col min="2055" max="2055" width="12.875" style="238" customWidth="1"/>
-    <col min="2056" max="2056" width="14.75" style="238" customWidth="1"/>
-    <col min="2057" max="2057" width="14.125" style="238" customWidth="1"/>
-    <col min="2058" max="2058" width="14.75" style="238" customWidth="1"/>
-    <col min="2059" max="2059" width="9.125" style="238"/>
-    <col min="2060" max="2070" width="0" style="238" hidden="1" customWidth="1"/>
-    <col min="2071" max="2304" width="9.125" style="238"/>
-    <col min="2305" max="2306" width="10" style="238" customWidth="1"/>
-    <col min="2307" max="2307" width="18" style="238" customWidth="1"/>
-    <col min="2308" max="2308" width="16" style="238" customWidth="1"/>
-    <col min="2309" max="2310" width="8.625" style="238" customWidth="1"/>
-    <col min="2311" max="2311" width="12.875" style="238" customWidth="1"/>
-    <col min="2312" max="2312" width="14.75" style="238" customWidth="1"/>
-    <col min="2313" max="2313" width="14.125" style="238" customWidth="1"/>
-    <col min="2314" max="2314" width="14.75" style="238" customWidth="1"/>
-    <col min="2315" max="2315" width="9.125" style="238"/>
-    <col min="2316" max="2326" width="0" style="238" hidden="1" customWidth="1"/>
-    <col min="2327" max="2560" width="9.125" style="238"/>
-    <col min="2561" max="2562" width="10" style="238" customWidth="1"/>
-    <col min="2563" max="2563" width="18" style="238" customWidth="1"/>
-    <col min="2564" max="2564" width="16" style="238" customWidth="1"/>
-    <col min="2565" max="2566" width="8.625" style="238" customWidth="1"/>
-    <col min="2567" max="2567" width="12.875" style="238" customWidth="1"/>
-    <col min="2568" max="2568" width="14.75" style="238" customWidth="1"/>
-    <col min="2569" max="2569" width="14.125" style="238" customWidth="1"/>
-    <col min="2570" max="2570" width="14.75" style="238" customWidth="1"/>
-    <col min="2571" max="2571" width="9.125" style="238"/>
-    <col min="2572" max="2582" width="0" style="238" hidden="1" customWidth="1"/>
-    <col min="2583" max="2816" width="9.125" style="238"/>
-    <col min="2817" max="2818" width="10" style="238" customWidth="1"/>
-    <col min="2819" max="2819" width="18" style="238" customWidth="1"/>
-    <col min="2820" max="2820" width="16" style="238" customWidth="1"/>
-    <col min="2821" max="2822" width="8.625" style="238" customWidth="1"/>
-    <col min="2823" max="2823" width="12.875" style="238" customWidth="1"/>
-    <col min="2824" max="2824" width="14.75" style="238" customWidth="1"/>
-    <col min="2825" max="2825" width="14.125" style="238" customWidth="1"/>
-    <col min="2826" max="2826" width="14.75" style="238" customWidth="1"/>
-    <col min="2827" max="2827" width="9.125" style="238"/>
-    <col min="2828" max="2838" width="0" style="238" hidden="1" customWidth="1"/>
-    <col min="2839" max="3072" width="9.125" style="238"/>
-    <col min="3073" max="3074" width="10" style="238" customWidth="1"/>
-    <col min="3075" max="3075" width="18" style="238" customWidth="1"/>
-    <col min="3076" max="3076" width="16" style="238" customWidth="1"/>
-    <col min="3077" max="3078" width="8.625" style="238" customWidth="1"/>
-    <col min="3079" max="3079" width="12.875" style="238" customWidth="1"/>
-    <col min="3080" max="3080" width="14.75" style="238" customWidth="1"/>
-    <col min="3081" max="3081" width="14.125" style="238" customWidth="1"/>
-    <col min="3082" max="3082" width="14.75" style="238" customWidth="1"/>
-    <col min="3083" max="3083" width="9.125" style="238"/>
-    <col min="3084" max="3094" width="0" style="238" hidden="1" customWidth="1"/>
-    <col min="3095" max="3328" width="9.125" style="238"/>
-    <col min="3329" max="3330" width="10" style="238" customWidth="1"/>
-    <col min="3331" max="3331" width="18" style="238" customWidth="1"/>
-    <col min="3332" max="3332" width="16" style="238" customWidth="1"/>
-    <col min="3333" max="3334" width="8.625" style="238" customWidth="1"/>
-    <col min="3335" max="3335" width="12.875" style="238" customWidth="1"/>
-    <col min="3336" max="3336" width="14.75" style="238" customWidth="1"/>
-    <col min="3337" max="3337" width="14.125" style="238" customWidth="1"/>
-    <col min="3338" max="3338" width="14.75" style="238" customWidth="1"/>
-    <col min="3339" max="3339" width="9.125" style="238"/>
-    <col min="3340" max="3350" width="0" style="238" hidden="1" customWidth="1"/>
-    <col min="3351" max="3584" width="9.125" style="238"/>
-    <col min="3585" max="3586" width="10" style="238" customWidth="1"/>
-    <col min="3587" max="3587" width="18" style="238" customWidth="1"/>
-    <col min="3588" max="3588" width="16" style="238" customWidth="1"/>
-    <col min="3589" max="3590" width="8.625" style="238" customWidth="1"/>
-    <col min="3591" max="3591" width="12.875" style="238" customWidth="1"/>
-    <col min="3592" max="3592" width="14.75" style="238" customWidth="1"/>
-    <col min="3593" max="3593" width="14.125" style="238" customWidth="1"/>
-    <col min="3594" max="3594" width="14.75" style="238" customWidth="1"/>
-    <col min="3595" max="3595" width="9.125" style="238"/>
-    <col min="3596" max="3606" width="0" style="238" hidden="1" customWidth="1"/>
-    <col min="3607" max="3840" width="9.125" style="238"/>
-    <col min="3841" max="3842" width="10" style="238" customWidth="1"/>
-    <col min="3843" max="3843" width="18" style="238" customWidth="1"/>
-    <col min="3844" max="3844" width="16" style="238" customWidth="1"/>
-    <col min="3845" max="3846" width="8.625" style="238" customWidth="1"/>
-    <col min="3847" max="3847" width="12.875" style="238" customWidth="1"/>
-    <col min="3848" max="3848" width="14.75" style="238" customWidth="1"/>
-    <col min="3849" max="3849" width="14.125" style="238" customWidth="1"/>
-    <col min="3850" max="3850" width="14.75" style="238" customWidth="1"/>
-    <col min="3851" max="3851" width="9.125" style="238"/>
-    <col min="3852" max="3862" width="0" style="238" hidden="1" customWidth="1"/>
-    <col min="3863" max="4096" width="9.125" style="238"/>
-    <col min="4097" max="4098" width="10" style="238" customWidth="1"/>
-    <col min="4099" max="4099" width="18" style="238" customWidth="1"/>
-    <col min="4100" max="4100" width="16" style="238" customWidth="1"/>
-    <col min="4101" max="4102" width="8.625" style="238" customWidth="1"/>
-    <col min="4103" max="4103" width="12.875" style="238" customWidth="1"/>
-    <col min="4104" max="4104" width="14.75" style="238" customWidth="1"/>
-    <col min="4105" max="4105" width="14.125" style="238" customWidth="1"/>
-    <col min="4106" max="4106" width="14.75" style="238" customWidth="1"/>
-    <col min="4107" max="4107" width="9.125" style="238"/>
-    <col min="4108" max="4118" width="0" style="238" hidden="1" customWidth="1"/>
-    <col min="4119" max="4352" width="9.125" style="238"/>
-    <col min="4353" max="4354" width="10" style="238" customWidth="1"/>
-    <col min="4355" max="4355" width="18" style="238" customWidth="1"/>
-    <col min="4356" max="4356" width="16" style="238" customWidth="1"/>
-    <col min="4357" max="4358" width="8.625" style="238" customWidth="1"/>
-    <col min="4359" max="4359" width="12.875" style="238" customWidth="1"/>
-    <col min="4360" max="4360" width="14.75" style="238" customWidth="1"/>
-    <col min="4361" max="4361" width="14.125" style="238" customWidth="1"/>
-    <col min="4362" max="4362" width="14.75" style="238" customWidth="1"/>
-    <col min="4363" max="4363" width="9.125" style="238"/>
-    <col min="4364" max="4374" width="0" style="238" hidden="1" customWidth="1"/>
-    <col min="4375" max="4608" width="9.125" style="238"/>
-    <col min="4609" max="4610" width="10" style="238" customWidth="1"/>
-    <col min="4611" max="4611" width="18" style="238" customWidth="1"/>
-    <col min="4612" max="4612" width="16" style="238" customWidth="1"/>
-    <col min="4613" max="4614" width="8.625" style="238" customWidth="1"/>
-    <col min="4615" max="4615" width="12.875" style="238" customWidth="1"/>
-    <col min="4616" max="4616" width="14.75" style="238" customWidth="1"/>
-    <col min="4617" max="4617" width="14.125" style="238" customWidth="1"/>
-    <col min="4618" max="4618" width="14.75" style="238" customWidth="1"/>
-    <col min="4619" max="4619" width="9.125" style="238"/>
-    <col min="4620" max="4630" width="0" style="238" hidden="1" customWidth="1"/>
-    <col min="4631" max="4864" width="9.125" style="238"/>
-    <col min="4865" max="4866" width="10" style="238" customWidth="1"/>
-    <col min="4867" max="4867" width="18" style="238" customWidth="1"/>
-    <col min="4868" max="4868" width="16" style="238" customWidth="1"/>
-    <col min="4869" max="4870" width="8.625" style="238" customWidth="1"/>
-    <col min="4871" max="4871" width="12.875" style="238" customWidth="1"/>
-    <col min="4872" max="4872" width="14.75" style="238" customWidth="1"/>
-    <col min="4873" max="4873" width="14.125" style="238" customWidth="1"/>
-    <col min="4874" max="4874" width="14.75" style="238" customWidth="1"/>
-    <col min="4875" max="4875" width="9.125" style="238"/>
-    <col min="4876" max="4886" width="0" style="238" hidden="1" customWidth="1"/>
-    <col min="4887" max="5120" width="9.125" style="238"/>
-    <col min="5121" max="5122" width="10" style="238" customWidth="1"/>
-    <col min="5123" max="5123" width="18" style="238" customWidth="1"/>
-    <col min="5124" max="5124" width="16" style="238" customWidth="1"/>
-    <col min="5125" max="5126" width="8.625" style="238" customWidth="1"/>
-    <col min="5127" max="5127" width="12.875" style="238" customWidth="1"/>
-    <col min="5128" max="5128" width="14.75" style="238" customWidth="1"/>
-    <col min="5129" max="5129" width="14.125" style="238" customWidth="1"/>
-    <col min="5130" max="5130" width="14.75" style="238" customWidth="1"/>
-    <col min="5131" max="5131" width="9.125" style="238"/>
-    <col min="5132" max="5142" width="0" style="238" hidden="1" customWidth="1"/>
-    <col min="5143" max="5376" width="9.125" style="238"/>
-    <col min="5377" max="5378" width="10" style="238" customWidth="1"/>
-    <col min="5379" max="5379" width="18" style="238" customWidth="1"/>
-    <col min="5380" max="5380" width="16" style="238" customWidth="1"/>
-    <col min="5381" max="5382" width="8.625" style="238" customWidth="1"/>
-    <col min="5383" max="5383" width="12.875" style="238" customWidth="1"/>
-    <col min="5384" max="5384" width="14.75" style="238" customWidth="1"/>
-    <col min="5385" max="5385" width="14.125" style="238" customWidth="1"/>
-    <col min="5386" max="5386" width="14.75" style="238" customWidth="1"/>
-    <col min="5387" max="5387" width="9.125" style="238"/>
-    <col min="5388" max="5398" width="0" style="238" hidden="1" customWidth="1"/>
-    <col min="5399" max="5632" width="9.125" style="238"/>
-    <col min="5633" max="5634" width="10" style="238" customWidth="1"/>
-    <col min="5635" max="5635" width="18" style="238" customWidth="1"/>
-    <col min="5636" max="5636" width="16" style="238" customWidth="1"/>
-    <col min="5637" max="5638" width="8.625" style="238" customWidth="1"/>
-    <col min="5639" max="5639" width="12.875" style="238" customWidth="1"/>
-    <col min="5640" max="5640" width="14.75" style="238" customWidth="1"/>
-    <col min="5641" max="5641" width="14.125" style="238" customWidth="1"/>
-    <col min="5642" max="5642" width="14.75" style="238" customWidth="1"/>
-    <col min="5643" max="5643" width="9.125" style="238"/>
-    <col min="5644" max="5654" width="0" style="238" hidden="1" customWidth="1"/>
-    <col min="5655" max="5888" width="9.125" style="238"/>
-    <col min="5889" max="5890" width="10" style="238" customWidth="1"/>
-    <col min="5891" max="5891" width="18" style="238" customWidth="1"/>
-    <col min="5892" max="5892" width="16" style="238" customWidth="1"/>
-    <col min="5893" max="5894" width="8.625" style="238" customWidth="1"/>
-    <col min="5895" max="5895" width="12.875" style="238" customWidth="1"/>
-    <col min="5896" max="5896" width="14.75" style="238" customWidth="1"/>
-    <col min="5897" max="5897" width="14.125" style="238" customWidth="1"/>
-    <col min="5898" max="5898" width="14.75" style="238" customWidth="1"/>
-    <col min="5899" max="5899" width="9.125" style="238"/>
-    <col min="5900" max="5910" width="0" style="238" hidden="1" customWidth="1"/>
-    <col min="5911" max="6144" width="9.125" style="238"/>
-    <col min="6145" max="6146" width="10" style="238" customWidth="1"/>
-    <col min="6147" max="6147" width="18" style="238" customWidth="1"/>
-    <col min="6148" max="6148" width="16" style="238" customWidth="1"/>
-    <col min="6149" max="6150" width="8.625" style="238" customWidth="1"/>
-    <col min="6151" max="6151" width="12.875" style="238" customWidth="1"/>
-    <col min="6152" max="6152" width="14.75" style="238" customWidth="1"/>
-    <col min="6153" max="6153" width="14.125" style="238" customWidth="1"/>
-    <col min="6154" max="6154" width="14.75" style="238" customWidth="1"/>
-    <col min="6155" max="6155" width="9.125" style="238"/>
-    <col min="6156" max="6166" width="0" style="238" hidden="1" customWidth="1"/>
-    <col min="6167" max="6400" width="9.125" style="238"/>
-    <col min="6401" max="6402" width="10" style="238" customWidth="1"/>
-    <col min="6403" max="6403" width="18" style="238" customWidth="1"/>
-    <col min="6404" max="6404" width="16" style="238" customWidth="1"/>
-    <col min="6405" max="6406" width="8.625" style="238" customWidth="1"/>
-    <col min="6407" max="6407" width="12.875" style="238" customWidth="1"/>
-    <col min="6408" max="6408" width="14.75" style="238" customWidth="1"/>
-    <col min="6409" max="6409" width="14.125" style="238" customWidth="1"/>
-    <col min="6410" max="6410" width="14.75" style="238" customWidth="1"/>
-    <col min="6411" max="6411" width="9.125" style="238"/>
-    <col min="6412" max="6422" width="0" style="238" hidden="1" customWidth="1"/>
-    <col min="6423" max="6656" width="9.125" style="238"/>
-    <col min="6657" max="6658" width="10" style="238" customWidth="1"/>
-    <col min="6659" max="6659" width="18" style="238" customWidth="1"/>
-    <col min="6660" max="6660" width="16" style="238" customWidth="1"/>
-    <col min="6661" max="6662" width="8.625" style="238" customWidth="1"/>
-    <col min="6663" max="6663" width="12.875" style="238" customWidth="1"/>
-    <col min="6664" max="6664" width="14.75" style="238" customWidth="1"/>
-    <col min="6665" max="6665" width="14.125" style="238" customWidth="1"/>
-    <col min="6666" max="6666" width="14.75" style="238" customWidth="1"/>
-    <col min="6667" max="6667" width="9.125" style="238"/>
-    <col min="6668" max="6678" width="0" style="238" hidden="1" customWidth="1"/>
-    <col min="6679" max="6912" width="9.125" style="238"/>
-    <col min="6913" max="6914" width="10" style="238" customWidth="1"/>
-    <col min="6915" max="6915" width="18" style="238" customWidth="1"/>
-    <col min="6916" max="6916" width="16" style="238" customWidth="1"/>
-    <col min="6917" max="6918" width="8.625" style="238" customWidth="1"/>
-    <col min="6919" max="6919" width="12.875" style="238" customWidth="1"/>
-    <col min="6920" max="6920" width="14.75" style="238" customWidth="1"/>
-    <col min="6921" max="6921" width="14.125" style="238" customWidth="1"/>
-    <col min="6922" max="6922" width="14.75" style="238" customWidth="1"/>
-    <col min="6923" max="6923" width="9.125" style="238"/>
-    <col min="6924" max="6934" width="0" style="238" hidden="1" customWidth="1"/>
-    <col min="6935" max="7168" width="9.125" style="238"/>
-    <col min="7169" max="7170" width="10" style="238" customWidth="1"/>
-    <col min="7171" max="7171" width="18" style="238" customWidth="1"/>
-    <col min="7172" max="7172" width="16" style="238" customWidth="1"/>
-    <col min="7173" max="7174" width="8.625" style="238" customWidth="1"/>
-    <col min="7175" max="7175" width="12.875" style="238" customWidth="1"/>
-    <col min="7176" max="7176" width="14.75" style="238" customWidth="1"/>
-    <col min="7177" max="7177" width="14.125" style="238" customWidth="1"/>
-    <col min="7178" max="7178" width="14.75" style="238" customWidth="1"/>
-    <col min="7179" max="7179" width="9.125" style="238"/>
-    <col min="7180" max="7190" width="0" style="238" hidden="1" customWidth="1"/>
-    <col min="7191" max="7424" width="9.125" style="238"/>
-    <col min="7425" max="7426" width="10" style="238" customWidth="1"/>
-    <col min="7427" max="7427" width="18" style="238" customWidth="1"/>
-    <col min="7428" max="7428" width="16" style="238" customWidth="1"/>
-    <col min="7429" max="7430" width="8.625" style="238" customWidth="1"/>
-    <col min="7431" max="7431" width="12.875" style="238" customWidth="1"/>
-    <col min="7432" max="7432" width="14.75" style="238" customWidth="1"/>
-    <col min="7433" max="7433" width="14.125" style="238" customWidth="1"/>
-    <col min="7434" max="7434" width="14.75" style="238" customWidth="1"/>
-    <col min="7435" max="7435" width="9.125" style="238"/>
-    <col min="7436" max="7446" width="0" style="238" hidden="1" customWidth="1"/>
-    <col min="7447" max="7680" width="9.125" style="238"/>
-    <col min="7681" max="7682" width="10" style="238" customWidth="1"/>
-    <col min="7683" max="7683" width="18" style="238" customWidth="1"/>
-    <col min="7684" max="7684" width="16" style="238" customWidth="1"/>
-    <col min="7685" max="7686" width="8.625" style="238" customWidth="1"/>
-    <col min="7687" max="7687" width="12.875" style="238" customWidth="1"/>
-    <col min="7688" max="7688" width="14.75" style="238" customWidth="1"/>
-    <col min="7689" max="7689" width="14.125" style="238" customWidth="1"/>
-    <col min="7690" max="7690" width="14.75" style="238" customWidth="1"/>
-    <col min="7691" max="7691" width="9.125" style="238"/>
-    <col min="7692" max="7702" width="0" style="238" hidden="1" customWidth="1"/>
-    <col min="7703" max="7936" width="9.125" style="238"/>
-    <col min="7937" max="7938" width="10" style="238" customWidth="1"/>
-    <col min="7939" max="7939" width="18" style="238" customWidth="1"/>
-    <col min="7940" max="7940" width="16" style="238" customWidth="1"/>
-    <col min="7941" max="7942" width="8.625" style="238" customWidth="1"/>
-    <col min="7943" max="7943" width="12.875" style="238" customWidth="1"/>
-    <col min="7944" max="7944" width="14.75" style="238" customWidth="1"/>
-    <col min="7945" max="7945" width="14.125" style="238" customWidth="1"/>
-    <col min="7946" max="7946" width="14.75" style="238" customWidth="1"/>
-    <col min="7947" max="7947" width="9.125" style="238"/>
-    <col min="7948" max="7958" width="0" style="238" hidden="1" customWidth="1"/>
-    <col min="7959" max="8192" width="9.125" style="238"/>
-    <col min="8193" max="8194" width="10" style="238" customWidth="1"/>
-    <col min="8195" max="8195" width="18" style="238" customWidth="1"/>
-    <col min="8196" max="8196" width="16" style="238" customWidth="1"/>
-    <col min="8197" max="8198" width="8.625" style="238" customWidth="1"/>
-    <col min="8199" max="8199" width="12.875" style="238" customWidth="1"/>
-    <col min="8200" max="8200" width="14.75" style="238" customWidth="1"/>
-    <col min="8201" max="8201" width="14.125" style="238" customWidth="1"/>
-    <col min="8202" max="8202" width="14.75" style="238" customWidth="1"/>
-    <col min="8203" max="8203" width="9.125" style="238"/>
-    <col min="8204" max="8214" width="0" style="238" hidden="1" customWidth="1"/>
-    <col min="8215" max="8448" width="9.125" style="238"/>
-    <col min="8449" max="8450" width="10" style="238" customWidth="1"/>
-    <col min="8451" max="8451" width="18" style="238" customWidth="1"/>
-    <col min="8452" max="8452" width="16" style="238" customWidth="1"/>
-    <col min="8453" max="8454" width="8.625" style="238" customWidth="1"/>
-    <col min="8455" max="8455" width="12.875" style="238" customWidth="1"/>
-    <col min="8456" max="8456" width="14.75" style="238" customWidth="1"/>
-    <col min="8457" max="8457" width="14.125" style="238" customWidth="1"/>
-    <col min="8458" max="8458" width="14.75" style="238" customWidth="1"/>
-    <col min="8459" max="8459" width="9.125" style="238"/>
-    <col min="8460" max="8470" width="0" style="238" hidden="1" customWidth="1"/>
-    <col min="8471" max="8704" width="9.125" style="238"/>
-    <col min="8705" max="8706" width="10" style="238" customWidth="1"/>
-    <col min="8707" max="8707" width="18" style="238" customWidth="1"/>
-    <col min="8708" max="8708" width="16" style="238" customWidth="1"/>
-    <col min="8709" max="8710" width="8.625" style="238" customWidth="1"/>
-    <col min="8711" max="8711" width="12.875" style="238" customWidth="1"/>
-    <col min="8712" max="8712" width="14.75" style="238" customWidth="1"/>
-    <col min="8713" max="8713" width="14.125" style="238" customWidth="1"/>
-    <col min="8714" max="8714" width="14.75" style="238" customWidth="1"/>
-    <col min="8715" max="8715" width="9.125" style="238"/>
-    <col min="8716" max="8726" width="0" style="238" hidden="1" customWidth="1"/>
-    <col min="8727" max="8960" width="9.125" style="238"/>
-    <col min="8961" max="8962" width="10" style="238" customWidth="1"/>
-    <col min="8963" max="8963" width="18" style="238" customWidth="1"/>
-    <col min="8964" max="8964" width="16" style="238" customWidth="1"/>
-    <col min="8965" max="8966" width="8.625" style="238" customWidth="1"/>
-    <col min="8967" max="8967" width="12.875" style="238" customWidth="1"/>
-    <col min="8968" max="8968" width="14.75" style="238" customWidth="1"/>
-    <col min="8969" max="8969" width="14.125" style="238" customWidth="1"/>
-    <col min="8970" max="8970" width="14.75" style="238" customWidth="1"/>
-    <col min="8971" max="8971" width="9.125" style="238"/>
-    <col min="8972" max="8982" width="0" style="238" hidden="1" customWidth="1"/>
-    <col min="8983" max="9216" width="9.125" style="238"/>
-    <col min="9217" max="9218" width="10" style="238" customWidth="1"/>
-    <col min="9219" max="9219" width="18" style="238" customWidth="1"/>
-    <col min="9220" max="9220" width="16" style="238" customWidth="1"/>
-    <col min="9221" max="9222" width="8.625" style="238" customWidth="1"/>
-    <col min="9223" max="9223" width="12.875" style="238" customWidth="1"/>
-    <col min="9224" max="9224" width="14.75" style="238" customWidth="1"/>
-    <col min="9225" max="9225" width="14.125" style="238" customWidth="1"/>
-    <col min="9226" max="9226" width="14.75" style="238" customWidth="1"/>
-    <col min="9227" max="9227" width="9.125" style="238"/>
-    <col min="9228" max="9238" width="0" style="238" hidden="1" customWidth="1"/>
-    <col min="9239" max="9472" width="9.125" style="238"/>
-    <col min="9473" max="9474" width="10" style="238" customWidth="1"/>
-    <col min="9475" max="9475" width="18" style="238" customWidth="1"/>
-    <col min="9476" max="9476" width="16" style="238" customWidth="1"/>
-    <col min="9477" max="9478" width="8.625" style="238" customWidth="1"/>
-    <col min="9479" max="9479" width="12.875" style="238" customWidth="1"/>
-    <col min="9480" max="9480" width="14.75" style="238" customWidth="1"/>
-    <col min="9481" max="9481" width="14.125" style="238" customWidth="1"/>
-    <col min="9482" max="9482" width="14.75" style="238" customWidth="1"/>
-    <col min="9483" max="9483" width="9.125" style="238"/>
-    <col min="9484" max="9494" width="0" style="238" hidden="1" customWidth="1"/>
-    <col min="9495" max="9728" width="9.125" style="238"/>
-    <col min="9729" max="9730" width="10" style="238" customWidth="1"/>
-    <col min="9731" max="9731" width="18" style="238" customWidth="1"/>
-    <col min="9732" max="9732" width="16" style="238" customWidth="1"/>
-    <col min="9733" max="9734" width="8.625" style="238" customWidth="1"/>
-    <col min="9735" max="9735" width="12.875" style="238" customWidth="1"/>
-    <col min="9736" max="9736" width="14.75" style="238" customWidth="1"/>
-    <col min="9737" max="9737" width="14.125" style="238" customWidth="1"/>
-    <col min="9738" max="9738" width="14.75" style="238" customWidth="1"/>
-    <col min="9739" max="9739" width="9.125" style="238"/>
-    <col min="9740" max="9750" width="0" style="238" hidden="1" customWidth="1"/>
-    <col min="9751" max="9984" width="9.125" style="238"/>
-    <col min="9985" max="9986" width="10" style="238" customWidth="1"/>
-    <col min="9987" max="9987" width="18" style="238" customWidth="1"/>
-    <col min="9988" max="9988" width="16" style="238" customWidth="1"/>
-    <col min="9989" max="9990" width="8.625" style="238" customWidth="1"/>
-    <col min="9991" max="9991" width="12.875" style="238" customWidth="1"/>
-    <col min="9992" max="9992" width="14.75" style="238" customWidth="1"/>
-    <col min="9993" max="9993" width="14.125" style="238" customWidth="1"/>
-    <col min="9994" max="9994" width="14.75" style="238" customWidth="1"/>
-    <col min="9995" max="9995" width="9.125" style="238"/>
-    <col min="9996" max="10006" width="0" style="238" hidden="1" customWidth="1"/>
-    <col min="10007" max="10240" width="9.125" style="238"/>
-    <col min="10241" max="10242" width="10" style="238" customWidth="1"/>
-    <col min="10243" max="10243" width="18" style="238" customWidth="1"/>
-    <col min="10244" max="10244" width="16" style="238" customWidth="1"/>
-    <col min="10245" max="10246" width="8.625" style="238" customWidth="1"/>
-    <col min="10247" max="10247" width="12.875" style="238" customWidth="1"/>
-    <col min="10248" max="10248" width="14.75" style="238" customWidth="1"/>
-    <col min="10249" max="10249" width="14.125" style="238" customWidth="1"/>
-    <col min="10250" max="10250" width="14.75" style="238" customWidth="1"/>
-    <col min="10251" max="10251" width="9.125" style="238"/>
-    <col min="10252" max="10262" width="0" style="238" hidden="1" customWidth="1"/>
-    <col min="10263" max="10496" width="9.125" style="238"/>
-    <col min="10497" max="10498" width="10" style="238" customWidth="1"/>
-    <col min="10499" max="10499" width="18" style="238" customWidth="1"/>
-    <col min="10500" max="10500" width="16" style="238" customWidth="1"/>
-    <col min="10501" max="10502" width="8.625" style="238" customWidth="1"/>
-    <col min="10503" max="10503" width="12.875" style="238" customWidth="1"/>
-    <col min="10504" max="10504" width="14.75" style="238" customWidth="1"/>
-    <col min="10505" max="10505" width="14.125" style="238" customWidth="1"/>
-    <col min="10506" max="10506" width="14.75" style="238" customWidth="1"/>
-    <col min="10507" max="10507" width="9.125" style="238"/>
-    <col min="10508" max="10518" width="0" style="238" hidden="1" customWidth="1"/>
-    <col min="10519" max="10752" width="9.125" style="238"/>
-    <col min="10753" max="10754" width="10" style="238" customWidth="1"/>
-    <col min="10755" max="10755" width="18" style="238" customWidth="1"/>
-    <col min="10756" max="10756" width="16" style="238" customWidth="1"/>
-    <col min="10757" max="10758" width="8.625" style="238" customWidth="1"/>
-    <col min="10759" max="10759" width="12.875" style="238" customWidth="1"/>
-    <col min="10760" max="10760" width="14.75" style="238" customWidth="1"/>
-    <col min="10761" max="10761" width="14.125" style="238" customWidth="1"/>
-    <col min="10762" max="10762" width="14.75" style="238" customWidth="1"/>
-    <col min="10763" max="10763" width="9.125" style="238"/>
-    <col min="10764" max="10774" width="0" style="238" hidden="1" customWidth="1"/>
-    <col min="10775" max="11008" width="9.125" style="238"/>
-    <col min="11009" max="11010" width="10" style="238" customWidth="1"/>
-    <col min="11011" max="11011" width="18" style="238" customWidth="1"/>
-    <col min="11012" max="11012" width="16" style="238" customWidth="1"/>
-    <col min="11013" max="11014" width="8.625" style="238" customWidth="1"/>
-    <col min="11015" max="11015" width="12.875" style="238" customWidth="1"/>
-    <col min="11016" max="11016" width="14.75" style="238" customWidth="1"/>
-    <col min="11017" max="11017" width="14.125" style="238" customWidth="1"/>
-    <col min="11018" max="11018" width="14.75" style="238" customWidth="1"/>
-    <col min="11019" max="11019" width="9.125" style="238"/>
-    <col min="11020" max="11030" width="0" style="238" hidden="1" customWidth="1"/>
-    <col min="11031" max="11264" width="9.125" style="238"/>
-    <col min="11265" max="11266" width="10" style="238" customWidth="1"/>
-    <col min="11267" max="11267" width="18" style="238" customWidth="1"/>
-    <col min="11268" max="11268" width="16" style="238" customWidth="1"/>
-    <col min="11269" max="11270" width="8.625" style="238" customWidth="1"/>
-    <col min="11271" max="11271" width="12.875" style="238" customWidth="1"/>
-    <col min="11272" max="11272" width="14.75" style="238" customWidth="1"/>
-    <col min="11273" max="11273" width="14.125" style="238" customWidth="1"/>
-    <col min="11274" max="11274" width="14.75" style="238" customWidth="1"/>
-    <col min="11275" max="11275" width="9.125" style="238"/>
-    <col min="11276" max="11286" width="0" style="238" hidden="1" customWidth="1"/>
-    <col min="11287" max="11520" width="9.125" style="238"/>
-    <col min="11521" max="11522" width="10" style="238" customWidth="1"/>
-    <col min="11523" max="11523" width="18" style="238" customWidth="1"/>
-    <col min="11524" max="11524" width="16" style="238" customWidth="1"/>
-    <col min="11525" max="11526" width="8.625" style="238" customWidth="1"/>
-    <col min="11527" max="11527" width="12.875" style="238" customWidth="1"/>
-    <col min="11528" max="11528" width="14.75" style="238" customWidth="1"/>
-    <col min="11529" max="11529" width="14.125" style="238" customWidth="1"/>
-    <col min="11530" max="11530" width="14.75" style="238" customWidth="1"/>
-    <col min="11531" max="11531" width="9.125" style="238"/>
-    <col min="11532" max="11542" width="0" style="238" hidden="1" customWidth="1"/>
-    <col min="11543" max="11776" width="9.125" style="238"/>
-    <col min="11777" max="11778" width="10" style="238" customWidth="1"/>
-    <col min="11779" max="11779" width="18" style="238" customWidth="1"/>
-    <col min="11780" max="11780" width="16" style="238" customWidth="1"/>
-    <col min="11781" max="11782" width="8.625" style="238" customWidth="1"/>
-    <col min="11783" max="11783" width="12.875" style="238" customWidth="1"/>
-    <col min="11784" max="11784" width="14.75" style="238" customWidth="1"/>
-    <col min="11785" max="11785" width="14.125" style="238" customWidth="1"/>
-    <col min="11786" max="11786" width="14.75" style="238" customWidth="1"/>
-    <col min="11787" max="11787" width="9.125" style="238"/>
-    <col min="11788" max="11798" width="0" style="238" hidden="1" customWidth="1"/>
-    <col min="11799" max="12032" width="9.125" style="238"/>
-    <col min="12033" max="12034" width="10" style="238" customWidth="1"/>
-    <col min="12035" max="12035" width="18" style="238" customWidth="1"/>
-    <col min="12036" max="12036" width="16" style="238" customWidth="1"/>
-    <col min="12037" max="12038" width="8.625" style="238" customWidth="1"/>
-    <col min="12039" max="12039" width="12.875" style="238" customWidth="1"/>
-    <col min="12040" max="12040" width="14.75" style="238" customWidth="1"/>
-    <col min="12041" max="12041" width="14.125" style="238" customWidth="1"/>
-    <col min="12042" max="12042" width="14.75" style="238" customWidth="1"/>
-    <col min="12043" max="12043" width="9.125" style="238"/>
-    <col min="12044" max="12054" width="0" style="238" hidden="1" customWidth="1"/>
-    <col min="12055" max="12288" width="9.125" style="238"/>
-    <col min="12289" max="12290" width="10" style="238" customWidth="1"/>
-    <col min="12291" max="12291" width="18" style="238" customWidth="1"/>
-    <col min="12292" max="12292" width="16" style="238" customWidth="1"/>
-    <col min="12293" max="12294" width="8.625" style="238" customWidth="1"/>
-    <col min="12295" max="12295" width="12.875" style="238" customWidth="1"/>
-    <col min="12296" max="12296" width="14.75" style="238" customWidth="1"/>
-    <col min="12297" max="12297" width="14.125" style="238" customWidth="1"/>
-    <col min="12298" max="12298" width="14.75" style="238" customWidth="1"/>
-    <col min="12299" max="12299" width="9.125" style="238"/>
-    <col min="12300" max="12310" width="0" style="238" hidden="1" customWidth="1"/>
-    <col min="12311" max="12544" width="9.125" style="238"/>
-    <col min="12545" max="12546" width="10" style="238" customWidth="1"/>
-    <col min="12547" max="12547" width="18" style="238" customWidth="1"/>
-    <col min="12548" max="12548" width="16" style="238" customWidth="1"/>
-    <col min="12549" max="12550" width="8.625" style="238" customWidth="1"/>
-    <col min="12551" max="12551" width="12.875" style="238" customWidth="1"/>
-    <col min="12552" max="12552" width="14.75" style="238" customWidth="1"/>
-    <col min="12553" max="12553" width="14.125" style="238" customWidth="1"/>
-    <col min="12554" max="12554" width="14.75" style="238" customWidth="1"/>
-    <col min="12555" max="12555" width="9.125" style="238"/>
-    <col min="12556" max="12566" width="0" style="238" hidden="1" customWidth="1"/>
-    <col min="12567" max="12800" width="9.125" style="238"/>
-    <col min="12801" max="12802" width="10" style="238" customWidth="1"/>
-    <col min="12803" max="12803" width="18" style="238" customWidth="1"/>
-    <col min="12804" max="12804" width="16" style="238" customWidth="1"/>
-    <col min="12805" max="12806" width="8.625" style="238" customWidth="1"/>
-    <col min="12807" max="12807" width="12.875" style="238" customWidth="1"/>
-    <col min="12808" max="12808" width="14.75" style="238" customWidth="1"/>
-    <col min="12809" max="12809" width="14.125" style="238" customWidth="1"/>
-    <col min="12810" max="12810" width="14.75" style="238" customWidth="1"/>
-    <col min="12811" max="12811" width="9.125" style="238"/>
-    <col min="12812" max="12822" width="0" style="238" hidden="1" customWidth="1"/>
-    <col min="12823" max="13056" width="9.125" style="238"/>
-    <col min="13057" max="13058" width="10" style="238" customWidth="1"/>
-    <col min="13059" max="13059" width="18" style="238" customWidth="1"/>
-    <col min="13060" max="13060" width="16" style="238" customWidth="1"/>
-    <col min="13061" max="13062" width="8.625" style="238" customWidth="1"/>
-    <col min="13063" max="13063" width="12.875" style="238" customWidth="1"/>
-    <col min="13064" max="13064" width="14.75" style="238" customWidth="1"/>
-    <col min="13065" max="13065" width="14.125" style="238" customWidth="1"/>
-    <col min="13066" max="13066" width="14.75" style="238" customWidth="1"/>
-    <col min="13067" max="13067" width="9.125" style="238"/>
-    <col min="13068" max="13078" width="0" style="238" hidden="1" customWidth="1"/>
-    <col min="13079" max="13312" width="9.125" style="238"/>
-    <col min="13313" max="13314" width="10" style="238" customWidth="1"/>
-    <col min="13315" max="13315" width="18" style="238" customWidth="1"/>
-    <col min="13316" max="13316" width="16" style="238" customWidth="1"/>
-    <col min="13317" max="13318" width="8.625" style="238" customWidth="1"/>
-    <col min="13319" max="13319" width="12.875" style="238" customWidth="1"/>
-    <col min="13320" max="13320" width="14.75" style="238" customWidth="1"/>
-    <col min="13321" max="13321" width="14.125" style="238" customWidth="1"/>
-    <col min="13322" max="13322" width="14.75" style="238" customWidth="1"/>
-    <col min="13323" max="13323" width="9.125" style="238"/>
-    <col min="13324" max="13334" width="0" style="238" hidden="1" customWidth="1"/>
-    <col min="13335" max="13568" width="9.125" style="238"/>
-    <col min="13569" max="13570" width="10" style="238" customWidth="1"/>
-    <col min="13571" max="13571" width="18" style="238" customWidth="1"/>
-    <col min="13572" max="13572" width="16" style="238" customWidth="1"/>
-    <col min="13573" max="13574" width="8.625" style="238" customWidth="1"/>
-    <col min="13575" max="13575" width="12.875" style="238" customWidth="1"/>
-    <col min="13576" max="13576" width="14.75" style="238" customWidth="1"/>
-    <col min="13577" max="13577" width="14.125" style="238" customWidth="1"/>
-    <col min="13578" max="13578" width="14.75" style="238" customWidth="1"/>
-    <col min="13579" max="13579" width="9.125" style="238"/>
-    <col min="13580" max="13590" width="0" style="238" hidden="1" customWidth="1"/>
-    <col min="13591" max="13824" width="9.125" style="238"/>
-    <col min="13825" max="13826" width="10" style="238" customWidth="1"/>
-    <col min="13827" max="13827" width="18" style="238" customWidth="1"/>
-    <col min="13828" max="13828" width="16" style="238" customWidth="1"/>
-    <col min="13829" max="13830" width="8.625" style="238" customWidth="1"/>
-    <col min="13831" max="13831" width="12.875" style="238" customWidth="1"/>
-    <col min="13832" max="13832" width="14.75" style="238" customWidth="1"/>
-    <col min="13833" max="13833" width="14.125" style="238" customWidth="1"/>
-    <col min="13834" max="13834" width="14.75" style="238" customWidth="1"/>
-    <col min="13835" max="13835" width="9.125" style="238"/>
-    <col min="13836" max="13846" width="0" style="238" hidden="1" customWidth="1"/>
-    <col min="13847" max="14080" width="9.125" style="238"/>
-    <col min="14081" max="14082" width="10" style="238" customWidth="1"/>
-    <col min="14083" max="14083" width="18" style="238" customWidth="1"/>
-    <col min="14084" max="14084" width="16" style="238" customWidth="1"/>
-    <col min="14085" max="14086" width="8.625" style="238" customWidth="1"/>
-    <col min="14087" max="14087" width="12.875" style="238" customWidth="1"/>
-    <col min="14088" max="14088" width="14.75" style="238" customWidth="1"/>
-    <col min="14089" max="14089" width="14.125" style="238" customWidth="1"/>
-    <col min="14090" max="14090" width="14.75" style="238" customWidth="1"/>
-    <col min="14091" max="14091" width="9.125" style="238"/>
-    <col min="14092" max="14102" width="0" style="238" hidden="1" customWidth="1"/>
-    <col min="14103" max="14336" width="9.125" style="238"/>
-    <col min="14337" max="14338" width="10" style="238" customWidth="1"/>
-    <col min="14339" max="14339" width="18" style="238" customWidth="1"/>
-    <col min="14340" max="14340" width="16" style="238" customWidth="1"/>
-    <col min="14341" max="14342" width="8.625" style="238" customWidth="1"/>
-    <col min="14343" max="14343" width="12.875" style="238" customWidth="1"/>
-    <col min="14344" max="14344" width="14.75" style="238" customWidth="1"/>
-    <col min="14345" max="14345" width="14.125" style="238" customWidth="1"/>
-    <col min="14346" max="14346" width="14.75" style="238" customWidth="1"/>
-    <col min="14347" max="14347" width="9.125" style="238"/>
-    <col min="14348" max="14358" width="0" style="238" hidden="1" customWidth="1"/>
-    <col min="14359" max="14592" width="9.125" style="238"/>
-    <col min="14593" max="14594" width="10" style="238" customWidth="1"/>
-    <col min="14595" max="14595" width="18" style="238" customWidth="1"/>
-    <col min="14596" max="14596" width="16" style="238" customWidth="1"/>
-    <col min="14597" max="14598" width="8.625" style="238" customWidth="1"/>
-    <col min="14599" max="14599" width="12.875" style="238" customWidth="1"/>
-    <col min="14600" max="14600" width="14.75" style="238" customWidth="1"/>
-    <col min="14601" max="14601" width="14.125" style="238" customWidth="1"/>
-    <col min="14602" max="14602" width="14.75" style="238" customWidth="1"/>
-    <col min="14603" max="14603" width="9.125" style="238"/>
-    <col min="14604" max="14614" width="0" style="238" hidden="1" customWidth="1"/>
-    <col min="14615" max="14848" width="9.125" style="238"/>
-    <col min="14849" max="14850" width="10" style="238" customWidth="1"/>
-    <col min="14851" max="14851" width="18" style="238" customWidth="1"/>
-    <col min="14852" max="14852" width="16" style="238" customWidth="1"/>
-    <col min="14853" max="14854" width="8.625" style="238" customWidth="1"/>
-    <col min="14855" max="14855" width="12.875" style="238" customWidth="1"/>
-    <col min="14856" max="14856" width="14.75" style="238" customWidth="1"/>
-    <col min="14857" max="14857" width="14.125" style="238" customWidth="1"/>
-    <col min="14858" max="14858" width="14.75" style="238" customWidth="1"/>
-    <col min="14859" max="14859" width="9.125" style="238"/>
-    <col min="14860" max="14870" width="0" style="238" hidden="1" customWidth="1"/>
-    <col min="14871" max="15104" width="9.125" style="238"/>
-    <col min="15105" max="15106" width="10" style="238" customWidth="1"/>
-    <col min="15107" max="15107" width="18" style="238" customWidth="1"/>
-    <col min="15108" max="15108" width="16" style="238" customWidth="1"/>
-    <col min="15109" max="15110" width="8.625" style="238" customWidth="1"/>
-    <col min="15111" max="15111" width="12.875" style="238" customWidth="1"/>
-    <col min="15112" max="15112" width="14.75" style="238" customWidth="1"/>
-    <col min="15113" max="15113" width="14.125" style="238" customWidth="1"/>
-    <col min="15114" max="15114" width="14.75" style="238" customWidth="1"/>
-    <col min="15115" max="15115" width="9.125" style="238"/>
-    <col min="15116" max="15126" width="0" style="238" hidden="1" customWidth="1"/>
-    <col min="15127" max="15360" width="9.125" style="238"/>
-    <col min="15361" max="15362" width="10" style="238" customWidth="1"/>
-    <col min="15363" max="15363" width="18" style="238" customWidth="1"/>
-    <col min="15364" max="15364" width="16" style="238" customWidth="1"/>
-    <col min="15365" max="15366" width="8.625" style="238" customWidth="1"/>
-    <col min="15367" max="15367" width="12.875" style="238" customWidth="1"/>
-    <col min="15368" max="15368" width="14.75" style="238" customWidth="1"/>
-    <col min="15369" max="15369" width="14.125" style="238" customWidth="1"/>
-    <col min="15370" max="15370" width="14.75" style="238" customWidth="1"/>
-    <col min="15371" max="15371" width="9.125" style="238"/>
-    <col min="15372" max="15382" width="0" style="238" hidden="1" customWidth="1"/>
-    <col min="15383" max="15616" width="9.125" style="238"/>
-    <col min="15617" max="15618" width="10" style="238" customWidth="1"/>
-    <col min="15619" max="15619" width="18" style="238" customWidth="1"/>
-    <col min="15620" max="15620" width="16" style="238" customWidth="1"/>
-    <col min="15621" max="15622" width="8.625" style="238" customWidth="1"/>
-    <col min="15623" max="15623" width="12.875" style="238" customWidth="1"/>
-    <col min="15624" max="15624" width="14.75" style="238" customWidth="1"/>
-    <col min="15625" max="15625" width="14.125" style="238" customWidth="1"/>
-    <col min="15626" max="15626" width="14.75" style="238" customWidth="1"/>
-    <col min="15627" max="15627" width="9.125" style="238"/>
-    <col min="15628" max="15638" width="0" style="238" hidden="1" customWidth="1"/>
-    <col min="15639" max="15872" width="9.125" style="238"/>
-    <col min="15873" max="15874" width="10" style="238" customWidth="1"/>
-    <col min="15875" max="15875" width="18" style="238" customWidth="1"/>
-    <col min="15876" max="15876" width="16" style="238" customWidth="1"/>
-    <col min="15877" max="15878" width="8.625" style="238" customWidth="1"/>
-    <col min="15879" max="15879" width="12.875" style="238" customWidth="1"/>
-    <col min="15880" max="15880" width="14.75" style="238" customWidth="1"/>
-    <col min="15881" max="15881" width="14.125" style="238" customWidth="1"/>
-    <col min="15882" max="15882" width="14.75" style="238" customWidth="1"/>
-    <col min="15883" max="15883" width="9.125" style="238"/>
-    <col min="15884" max="15894" width="0" style="238" hidden="1" customWidth="1"/>
-    <col min="15895" max="16128" width="9.125" style="238"/>
-    <col min="16129" max="16130" width="10" style="238" customWidth="1"/>
-    <col min="16131" max="16131" width="18" style="238" customWidth="1"/>
-    <col min="16132" max="16132" width="16" style="238" customWidth="1"/>
-    <col min="16133" max="16134" width="8.625" style="238" customWidth="1"/>
-    <col min="16135" max="16135" width="12.875" style="238" customWidth="1"/>
-    <col min="16136" max="16136" width="14.75" style="238" customWidth="1"/>
-    <col min="16137" max="16137" width="14.125" style="238" customWidth="1"/>
-    <col min="16138" max="16138" width="14.75" style="238" customWidth="1"/>
-    <col min="16139" max="16139" width="9.125" style="238"/>
-    <col min="16140" max="16150" width="0" style="238" hidden="1" customWidth="1"/>
-    <col min="16151" max="16384" width="9.125" style="238"/>
+    <col min="19" max="19" width="17.75" style="237" hidden="1" customWidth="1"/>
+    <col min="20" max="22" width="0" style="237" hidden="1" customWidth="1"/>
+    <col min="23" max="256" width="9.125" style="237"/>
+    <col min="257" max="258" width="10" style="237" customWidth="1"/>
+    <col min="259" max="259" width="18" style="237" customWidth="1"/>
+    <col min="260" max="260" width="16" style="237" customWidth="1"/>
+    <col min="261" max="262" width="8.625" style="237" customWidth="1"/>
+    <col min="263" max="263" width="12.875" style="237" customWidth="1"/>
+    <col min="264" max="264" width="14.75" style="237" customWidth="1"/>
+    <col min="265" max="265" width="14.125" style="237" customWidth="1"/>
+    <col min="266" max="266" width="14.75" style="237" customWidth="1"/>
+    <col min="267" max="267" width="9.125" style="237"/>
+    <col min="268" max="278" width="0" style="237" hidden="1" customWidth="1"/>
+    <col min="279" max="512" width="9.125" style="237"/>
+    <col min="513" max="514" width="10" style="237" customWidth="1"/>
+    <col min="515" max="515" width="18" style="237" customWidth="1"/>
+    <col min="516" max="516" width="16" style="237" customWidth="1"/>
+    <col min="517" max="518" width="8.625" style="237" customWidth="1"/>
+    <col min="519" max="519" width="12.875" style="237" customWidth="1"/>
+    <col min="520" max="520" width="14.75" style="237" customWidth="1"/>
+    <col min="521" max="521" width="14.125" style="237" customWidth="1"/>
+    <col min="522" max="522" width="14.75" style="237" customWidth="1"/>
+    <col min="523" max="523" width="9.125" style="237"/>
+    <col min="524" max="534" width="0" style="237" hidden="1" customWidth="1"/>
+    <col min="535" max="768" width="9.125" style="237"/>
+    <col min="769" max="770" width="10" style="237" customWidth="1"/>
+    <col min="771" max="771" width="18" style="237" customWidth="1"/>
+    <col min="772" max="772" width="16" style="237" customWidth="1"/>
+    <col min="773" max="774" width="8.625" style="237" customWidth="1"/>
+    <col min="775" max="775" width="12.875" style="237" customWidth="1"/>
+    <col min="776" max="776" width="14.75" style="237" customWidth="1"/>
+    <col min="777" max="777" width="14.125" style="237" customWidth="1"/>
+    <col min="778" max="778" width="14.75" style="237" customWidth="1"/>
+    <col min="779" max="779" width="9.125" style="237"/>
+    <col min="780" max="790" width="0" style="237" hidden="1" customWidth="1"/>
+    <col min="791" max="1024" width="9.125" style="237"/>
+    <col min="1025" max="1026" width="10" style="237" customWidth="1"/>
+    <col min="1027" max="1027" width="18" style="237" customWidth="1"/>
+    <col min="1028" max="1028" width="16" style="237" customWidth="1"/>
+    <col min="1029" max="1030" width="8.625" style="237" customWidth="1"/>
+    <col min="1031" max="1031" width="12.875" style="237" customWidth="1"/>
+    <col min="1032" max="1032" width="14.75" style="237" customWidth="1"/>
+    <col min="1033" max="1033" width="14.125" style="237" customWidth="1"/>
+    <col min="1034" max="1034" width="14.75" style="237" customWidth="1"/>
+    <col min="1035" max="1035" width="9.125" style="237"/>
+    <col min="1036" max="1046" width="0" style="237" hidden="1" customWidth="1"/>
+    <col min="1047" max="1280" width="9.125" style="237"/>
+    <col min="1281" max="1282" width="10" style="237" customWidth="1"/>
+    <col min="1283" max="1283" width="18" style="237" customWidth="1"/>
+    <col min="1284" max="1284" width="16" style="237" customWidth="1"/>
+    <col min="1285" max="1286" width="8.625" style="237" customWidth="1"/>
+    <col min="1287" max="1287" width="12.875" style="237" customWidth="1"/>
+    <col min="1288" max="1288" width="14.75" style="237" customWidth="1"/>
+    <col min="1289" max="1289" width="14.125" style="237" customWidth="1"/>
+    <col min="1290" max="1290" width="14.75" style="237" customWidth="1"/>
+    <col min="1291" max="1291" width="9.125" style="237"/>
+    <col min="1292" max="1302" width="0" style="237" hidden="1" customWidth="1"/>
+    <col min="1303" max="1536" width="9.125" style="237"/>
+    <col min="1537" max="1538" width="10" style="237" customWidth="1"/>
+    <col min="1539" max="1539" width="18" style="237" customWidth="1"/>
+    <col min="1540" max="1540" width="16" style="237" customWidth="1"/>
+    <col min="1541" max="1542" width="8.625" style="237" customWidth="1"/>
+    <col min="1543" max="1543" width="12.875" style="237" customWidth="1"/>
+    <col min="1544" max="1544" width="14.75" style="237" customWidth="1"/>
+    <col min="1545" max="1545" width="14.125" style="237" customWidth="1"/>
+    <col min="1546" max="1546" width="14.75" style="237" customWidth="1"/>
+    <col min="1547" max="1547" width="9.125" style="237"/>
+    <col min="1548" max="1558" width="0" style="237" hidden="1" customWidth="1"/>
+    <col min="1559" max="1792" width="9.125" style="237"/>
+    <col min="1793" max="1794" width="10" style="237" customWidth="1"/>
+    <col min="1795" max="1795" width="18" style="237" customWidth="1"/>
+    <col min="1796" max="1796" width="16" style="237" customWidth="1"/>
+    <col min="1797" max="1798" width="8.625" style="237" customWidth="1"/>
+    <col min="1799" max="1799" width="12.875" style="237" customWidth="1"/>
+    <col min="1800" max="1800" width="14.75" style="237" customWidth="1"/>
+    <col min="1801" max="1801" width="14.125" style="237" customWidth="1"/>
+    <col min="1802" max="1802" width="14.75" style="237" customWidth="1"/>
+    <col min="1803" max="1803" width="9.125" style="237"/>
+    <col min="1804" max="1814" width="0" style="237" hidden="1" customWidth="1"/>
+    <col min="1815" max="2048" width="9.125" style="237"/>
+    <col min="2049" max="2050" width="10" style="237" customWidth="1"/>
+    <col min="2051" max="2051" width="18" style="237" customWidth="1"/>
+    <col min="2052" max="2052" width="16" style="237" customWidth="1"/>
+    <col min="2053" max="2054" width="8.625" style="237" customWidth="1"/>
+    <col min="2055" max="2055" width="12.875" style="237" customWidth="1"/>
+    <col min="2056" max="2056" width="14.75" style="237" customWidth="1"/>
+    <col min="2057" max="2057" width="14.125" style="237" customWidth="1"/>
+    <col min="2058" max="2058" width="14.75" style="237" customWidth="1"/>
+    <col min="2059" max="2059" width="9.125" style="237"/>
+    <col min="2060" max="2070" width="0" style="237" hidden="1" customWidth="1"/>
+    <col min="2071" max="2304" width="9.125" style="237"/>
+    <col min="2305" max="2306" width="10" style="237" customWidth="1"/>
+    <col min="2307" max="2307" width="18" style="237" customWidth="1"/>
+    <col min="2308" max="2308" width="16" style="237" customWidth="1"/>
+    <col min="2309" max="2310" width="8.625" style="237" customWidth="1"/>
+    <col min="2311" max="2311" width="12.875" style="237" customWidth="1"/>
+    <col min="2312" max="2312" width="14.75" style="237" customWidth="1"/>
+    <col min="2313" max="2313" width="14.125" style="237" customWidth="1"/>
+    <col min="2314" max="2314" width="14.75" style="237" customWidth="1"/>
+    <col min="2315" max="2315" width="9.125" style="237"/>
+    <col min="2316" max="2326" width="0" style="237" hidden="1" customWidth="1"/>
+    <col min="2327" max="2560" width="9.125" style="237"/>
+    <col min="2561" max="2562" width="10" style="237" customWidth="1"/>
+    <col min="2563" max="2563" width="18" style="237" customWidth="1"/>
+    <col min="2564" max="2564" width="16" style="237" customWidth="1"/>
+    <col min="2565" max="2566" width="8.625" style="237" customWidth="1"/>
+    <col min="2567" max="2567" width="12.875" style="237" customWidth="1"/>
+    <col min="2568" max="2568" width="14.75" style="237" customWidth="1"/>
+    <col min="2569" max="2569" width="14.125" style="237" customWidth="1"/>
+    <col min="2570" max="2570" width="14.75" style="237" customWidth="1"/>
+    <col min="2571" max="2571" width="9.125" style="237"/>
+    <col min="2572" max="2582" width="0" style="237" hidden="1" customWidth="1"/>
+    <col min="2583" max="2816" width="9.125" style="237"/>
+    <col min="2817" max="2818" width="10" style="237" customWidth="1"/>
+    <col min="2819" max="2819" width="18" style="237" customWidth="1"/>
+    <col min="2820" max="2820" width="16" style="237" customWidth="1"/>
+    <col min="2821" max="2822" width="8.625" style="237" customWidth="1"/>
+    <col min="2823" max="2823" width="12.875" style="237" customWidth="1"/>
+    <col min="2824" max="2824" width="14.75" style="237" customWidth="1"/>
+    <col min="2825" max="2825" width="14.125" style="237" customWidth="1"/>
+    <col min="2826" max="2826" width="14.75" style="237" customWidth="1"/>
+    <col min="2827" max="2827" width="9.125" style="237"/>
+    <col min="2828" max="2838" width="0" style="237" hidden="1" customWidth="1"/>
+    <col min="2839" max="3072" width="9.125" style="237"/>
+    <col min="3073" max="3074" width="10" style="237" customWidth="1"/>
+    <col min="3075" max="3075" width="18" style="237" customWidth="1"/>
+    <col min="3076" max="3076" width="16" style="237" customWidth="1"/>
+    <col min="3077" max="3078" width="8.625" style="237" customWidth="1"/>
+    <col min="3079" max="3079" width="12.875" style="237" customWidth="1"/>
+    <col min="3080" max="3080" width="14.75" style="237" customWidth="1"/>
+    <col min="3081" max="3081" width="14.125" style="237" customWidth="1"/>
+    <col min="3082" max="3082" width="14.75" style="237" customWidth="1"/>
+    <col min="3083" max="3083" width="9.125" style="237"/>
+    <col min="3084" max="3094" width="0" style="237" hidden="1" customWidth="1"/>
+    <col min="3095" max="3328" width="9.125" style="237"/>
+    <col min="3329" max="3330" width="10" style="237" customWidth="1"/>
+    <col min="3331" max="3331" width="18" style="237" customWidth="1"/>
+    <col min="3332" max="3332" width="16" style="237" customWidth="1"/>
+    <col min="3333" max="3334" width="8.625" style="237" customWidth="1"/>
+    <col min="3335" max="3335" width="12.875" style="237" customWidth="1"/>
+    <col min="3336" max="3336" width="14.75" style="237" customWidth="1"/>
+    <col min="3337" max="3337" width="14.125" style="237" customWidth="1"/>
+    <col min="3338" max="3338" width="14.75" style="237" customWidth="1"/>
+    <col min="3339" max="3339" width="9.125" style="237"/>
+    <col min="3340" max="3350" width="0" style="237" hidden="1" customWidth="1"/>
+    <col min="3351" max="3584" width="9.125" style="237"/>
+    <col min="3585" max="3586" width="10" style="237" customWidth="1"/>
+    <col min="3587" max="3587" width="18" style="237" customWidth="1"/>
+    <col min="3588" max="3588" width="16" style="237" customWidth="1"/>
+    <col min="3589" max="3590" width="8.625" style="237" customWidth="1"/>
+    <col min="3591" max="3591" width="12.875" style="237" customWidth="1"/>
+    <col min="3592" max="3592" width="14.75" style="237" customWidth="1"/>
+    <col min="3593" max="3593" width="14.125" style="237" customWidth="1"/>
+    <col min="3594" max="3594" width="14.75" style="237" customWidth="1"/>
+    <col min="3595" max="3595" width="9.125" style="237"/>
+    <col min="3596" max="3606" width="0" style="237" hidden="1" customWidth="1"/>
+    <col min="3607" max="3840" width="9.125" style="237"/>
+    <col min="3841" max="3842" width="10" style="237" customWidth="1"/>
+    <col min="3843" max="3843" width="18" style="237" customWidth="1"/>
+    <col min="3844" max="3844" width="16" style="237" customWidth="1"/>
+    <col min="3845" max="3846" width="8.625" style="237" customWidth="1"/>
+    <col min="3847" max="3847" width="12.875" style="237" customWidth="1"/>
+    <col min="3848" max="3848" width="14.75" style="237" customWidth="1"/>
+    <col min="3849" max="3849" width="14.125" style="237" customWidth="1"/>
+    <col min="3850" max="3850" width="14.75" style="237" customWidth="1"/>
+    <col min="3851" max="3851" width="9.125" style="237"/>
+    <col min="3852" max="3862" width="0" style="237" hidden="1" customWidth="1"/>
+    <col min="3863" max="4096" width="9.125" style="237"/>
+    <col min="4097" max="4098" width="10" style="237" customWidth="1"/>
+    <col min="4099" max="4099" width="18" style="237" customWidth="1"/>
+    <col min="4100" max="4100" width="16" style="237" customWidth="1"/>
+    <col min="4101" max="4102" width="8.625" style="237" customWidth="1"/>
+    <col min="4103" max="4103" width="12.875" style="237" customWidth="1"/>
+    <col min="4104" max="4104" width="14.75" style="237" customWidth="1"/>
+    <col min="4105" max="4105" width="14.125" style="237" customWidth="1"/>
+    <col min="4106" max="4106" width="14.75" style="237" customWidth="1"/>
+    <col min="4107" max="4107" width="9.125" style="237"/>
+    <col min="4108" max="4118" width="0" style="237" hidden="1" customWidth="1"/>
+    <col min="4119" max="4352" width="9.125" style="237"/>
+    <col min="4353" max="4354" width="10" style="237" customWidth="1"/>
+    <col min="4355" max="4355" width="18" style="237" customWidth="1"/>
+    <col min="4356" max="4356" width="16" style="237" customWidth="1"/>
+    <col min="4357" max="4358" width="8.625" style="237" customWidth="1"/>
+    <col min="4359" max="4359" width="12.875" style="237" customWidth="1"/>
+    <col min="4360" max="4360" width="14.75" style="237" customWidth="1"/>
+    <col min="4361" max="4361" width="14.125" style="237" customWidth="1"/>
+    <col min="4362" max="4362" width="14.75" style="237" customWidth="1"/>
+    <col min="4363" max="4363" width="9.125" style="237"/>
+    <col min="4364" max="4374" width="0" style="237" hidden="1" customWidth="1"/>
+    <col min="4375" max="4608" width="9.125" style="237"/>
+    <col min="4609" max="4610" width="10" style="237" customWidth="1"/>
+    <col min="4611" max="4611" width="18" style="237" customWidth="1"/>
+    <col min="4612" max="4612" width="16" style="237" customWidth="1"/>
+    <col min="4613" max="4614" width="8.625" style="237" customWidth="1"/>
+    <col min="4615" max="4615" width="12.875" style="237" customWidth="1"/>
+    <col min="4616" max="4616" width="14.75" style="237" customWidth="1"/>
+    <col min="4617" max="4617" width="14.125" style="237" customWidth="1"/>
+    <col min="4618" max="4618" width="14.75" style="237" customWidth="1"/>
+    <col min="4619" max="4619" width="9.125" style="237"/>
+    <col min="4620" max="4630" width="0" style="237" hidden="1" customWidth="1"/>
+    <col min="4631" max="4864" width="9.125" style="237"/>
+    <col min="4865" max="4866" width="10" style="237" customWidth="1"/>
+    <col min="4867" max="4867" width="18" style="237" customWidth="1"/>
+    <col min="4868" max="4868" width="16" style="237" customWidth="1"/>
+    <col min="4869" max="4870" width="8.625" style="237" customWidth="1"/>
+    <col min="4871" max="4871" width="12.875" style="237" customWidth="1"/>
+    <col min="4872" max="4872" width="14.75" style="237" customWidth="1"/>
+    <col min="4873" max="4873" width="14.125" style="237" customWidth="1"/>
+    <col min="4874" max="4874" width="14.75" style="237" customWidth="1"/>
+    <col min="4875" max="4875" width="9.125" style="237"/>
+    <col min="4876" max="4886" width="0" style="237" hidden="1" customWidth="1"/>
+    <col min="4887" max="5120" width="9.125" style="237"/>
+    <col min="5121" max="5122" width="10" style="237" customWidth="1"/>
+    <col min="5123" max="5123" width="18" style="237" customWidth="1"/>
+    <col min="5124" max="5124" width="16" style="237" customWidth="1"/>
+    <col min="5125" max="5126" width="8.625" style="237" customWidth="1"/>
+    <col min="5127" max="5127" width="12.875" style="237" customWidth="1"/>
+    <col min="5128" max="5128" width="14.75" style="237" customWidth="1"/>
+    <col min="5129" max="5129" width="14.125" style="237" customWidth="1"/>
+    <col min="5130" max="5130" width="14.75" style="237" customWidth="1"/>
+    <col min="5131" max="5131" width="9.125" style="237"/>
+    <col min="5132" max="5142" width="0" style="237" hidden="1" customWidth="1"/>
+    <col min="5143" max="5376" width="9.125" style="237"/>
+    <col min="5377" max="5378" width="10" style="237" customWidth="1"/>
+    <col min="5379" max="5379" width="18" style="237" customWidth="1"/>
+    <col min="5380" max="5380" width="16" style="237" customWidth="1"/>
+    <col min="5381" max="5382" width="8.625" style="237" customWidth="1"/>
+    <col min="5383" max="5383" width="12.875" style="237" customWidth="1"/>
+    <col min="5384" max="5384" width="14.75" style="237" customWidth="1"/>
+    <col min="5385" max="5385" width="14.125" style="237" customWidth="1"/>
+    <col min="5386" max="5386" width="14.75" style="237" customWidth="1"/>
+    <col min="5387" max="5387" width="9.125" style="237"/>
+    <col min="5388" max="5398" width="0" style="237" hidden="1" customWidth="1"/>
+    <col min="5399" max="5632" width="9.125" style="237"/>
+    <col min="5633" max="5634" width="10" style="237" customWidth="1"/>
+    <col min="5635" max="5635" width="18" style="237" customWidth="1"/>
+    <col min="5636" max="5636" width="16" style="237" customWidth="1"/>
+    <col min="5637" max="5638" width="8.625" style="237" customWidth="1"/>
+    <col min="5639" max="5639" width="12.875" style="237" customWidth="1"/>
+    <col min="5640" max="5640" width="14.75" style="237" customWidth="1"/>
+    <col min="5641" max="5641" width="14.125" style="237" customWidth="1"/>
+    <col min="5642" max="5642" width="14.75" style="237" customWidth="1"/>
+    <col min="5643" max="5643" width="9.125" style="237"/>
+    <col min="5644" max="5654" width="0" style="237" hidden="1" customWidth="1"/>
+    <col min="5655" max="5888" width="9.125" style="237"/>
+    <col min="5889" max="5890" width="10" style="237" customWidth="1"/>
+    <col min="5891" max="5891" width="18" style="237" customWidth="1"/>
+    <col min="5892" max="5892" width="16" style="237" customWidth="1"/>
+    <col min="5893" max="5894" width="8.625" style="237" customWidth="1"/>
+    <col min="5895" max="5895" width="12.875" style="237" customWidth="1"/>
+    <col min="5896" max="5896" width="14.75" style="237" customWidth="1"/>
+    <col min="5897" max="5897" width="14.125" style="237" customWidth="1"/>
+    <col min="5898" max="5898" width="14.75" style="237" customWidth="1"/>
+    <col min="5899" max="5899" width="9.125" style="237"/>
+    <col min="5900" max="5910" width="0" style="237" hidden="1" customWidth="1"/>
+    <col min="5911" max="6144" width="9.125" style="237"/>
+    <col min="6145" max="6146" width="10" style="237" customWidth="1"/>
+    <col min="6147" max="6147" width="18" style="237" customWidth="1"/>
+    <col min="6148" max="6148" width="16" style="237" customWidth="1"/>
+    <col min="6149" max="6150" width="8.625" style="237" customWidth="1"/>
+    <col min="6151" max="6151" width="12.875" style="237" customWidth="1"/>
+    <col min="6152" max="6152" width="14.75" style="237" customWidth="1"/>
+    <col min="6153" max="6153" width="14.125" style="237" customWidth="1"/>
+    <col min="6154" max="6154" width="14.75" style="237" customWidth="1"/>
+    <col min="6155" max="6155" width="9.125" style="237"/>
+    <col min="6156" max="6166" width="0" style="237" hidden="1" customWidth="1"/>
+    <col min="6167" max="6400" width="9.125" style="237"/>
+    <col min="6401" max="6402" width="10" style="237" customWidth="1"/>
+    <col min="6403" max="6403" width="18" style="237" customWidth="1"/>
+    <col min="6404" max="6404" width="16" style="237" customWidth="1"/>
+    <col min="6405" max="6406" width="8.625" style="237" customWidth="1"/>
+    <col min="6407" max="6407" width="12.875" style="237" customWidth="1"/>
+    <col min="6408" max="6408" width="14.75" style="237" customWidth="1"/>
+    <col min="6409" max="6409" width="14.125" style="237" customWidth="1"/>
+    <col min="6410" max="6410" width="14.75" style="237" customWidth="1"/>
+    <col min="6411" max="6411" width="9.125" style="237"/>
+    <col min="6412" max="6422" width="0" style="237" hidden="1" customWidth="1"/>
+    <col min="6423" max="6656" width="9.125" style="237"/>
+    <col min="6657" max="6658" width="10" style="237" customWidth="1"/>
+    <col min="6659" max="6659" width="18" style="237" customWidth="1"/>
+    <col min="6660" max="6660" width="16" style="237" customWidth="1"/>
+    <col min="6661" max="6662" width="8.625" style="237" customWidth="1"/>
+    <col min="6663" max="6663" width="12.875" style="237" customWidth="1"/>
+    <col min="6664" max="6664" width="14.75" style="237" customWidth="1"/>
+    <col min="6665" max="6665" width="14.125" style="237" customWidth="1"/>
+    <col min="6666" max="6666" width="14.75" style="237" customWidth="1"/>
+    <col min="6667" max="6667" width="9.125" style="237"/>
+    <col min="6668" max="6678" width="0" style="237" hidden="1" customWidth="1"/>
+    <col min="6679" max="6912" width="9.125" style="237"/>
+    <col min="6913" max="6914" width="10" style="237" customWidth="1"/>
+    <col min="6915" max="6915" width="18" style="237" customWidth="1"/>
+    <col min="6916" max="6916" width="16" style="237" customWidth="1"/>
+    <col min="6917" max="6918" width="8.625" style="237" customWidth="1"/>
+    <col min="6919" max="6919" width="12.875" style="237" customWidth="1"/>
+    <col min="6920" max="6920" width="14.75" style="237" customWidth="1"/>
+    <col min="6921" max="6921" width="14.125" style="237" customWidth="1"/>
+    <col min="6922" max="6922" width="14.75" style="237" customWidth="1"/>
+    <col min="6923" max="6923" width="9.125" style="237"/>
+    <col min="6924" max="6934" width="0" style="237" hidden="1" customWidth="1"/>
+    <col min="6935" max="7168" width="9.125" style="237"/>
+    <col min="7169" max="7170" width="10" style="237" customWidth="1"/>
+    <col min="7171" max="7171" width="18" style="237" customWidth="1"/>
+    <col min="7172" max="7172" width="16" style="237" customWidth="1"/>
+    <col min="7173" max="7174" width="8.625" style="237" customWidth="1"/>
+    <col min="7175" max="7175" width="12.875" style="237" customWidth="1"/>
+    <col min="7176" max="7176" width="14.75" style="237" customWidth="1"/>
+    <col min="7177" max="7177" width="14.125" style="237" customWidth="1"/>
+    <col min="7178" max="7178" width="14.75" style="237" customWidth="1"/>
+    <col min="7179" max="7179" width="9.125" style="237"/>
+    <col min="7180" max="7190" width="0" style="237" hidden="1" customWidth="1"/>
+    <col min="7191" max="7424" width="9.125" style="237"/>
+    <col min="7425" max="7426" width="10" style="237" customWidth="1"/>
+    <col min="7427" max="7427" width="18" style="237" customWidth="1"/>
+    <col min="7428" max="7428" width="16" style="237" customWidth="1"/>
+    <col min="7429" max="7430" width="8.625" style="237" customWidth="1"/>
+    <col min="7431" max="7431" width="12.875" style="237" customWidth="1"/>
+    <col min="7432" max="7432" width="14.75" style="237" customWidth="1"/>
+    <col min="7433" max="7433" width="14.125" style="237" customWidth="1"/>
+    <col min="7434" max="7434" width="14.75" style="237" customWidth="1"/>
+    <col min="7435" max="7435" width="9.125" style="237"/>
+    <col min="7436" max="7446" width="0" style="237" hidden="1" customWidth="1"/>
+    <col min="7447" max="7680" width="9.125" style="237"/>
+    <col min="7681" max="7682" width="10" style="237" customWidth="1"/>
+    <col min="7683" max="7683" width="18" style="237" customWidth="1"/>
+    <col min="7684" max="7684" width="16" style="237" customWidth="1"/>
+    <col min="7685" max="7686" width="8.625" style="237" customWidth="1"/>
+    <col min="7687" max="7687" width="12.875" style="237" customWidth="1"/>
+    <col min="7688" max="7688" width="14.75" style="237" customWidth="1"/>
+    <col min="7689" max="7689" width="14.125" style="237" customWidth="1"/>
+    <col min="7690" max="7690" width="14.75" style="237" customWidth="1"/>
+    <col min="7691" max="7691" width="9.125" style="237"/>
+    <col min="7692" max="7702" width="0" style="237" hidden="1" customWidth="1"/>
+    <col min="7703" max="7936" width="9.125" style="237"/>
+    <col min="7937" max="7938" width="10" style="237" customWidth="1"/>
+    <col min="7939" max="7939" width="18" style="237" customWidth="1"/>
+    <col min="7940" max="7940" width="16" style="237" customWidth="1"/>
+    <col min="7941" max="7942" width="8.625" style="237" customWidth="1"/>
+    <col min="7943" max="7943" width="12.875" style="237" customWidth="1"/>
+    <col min="7944" max="7944" width="14.75" style="237" customWidth="1"/>
+    <col min="7945" max="7945" width="14.125" style="237" customWidth="1"/>
+    <col min="7946" max="7946" width="14.75" style="237" customWidth="1"/>
+    <col min="7947" max="7947" width="9.125" style="237"/>
+    <col min="7948" max="7958" width="0" style="237" hidden="1" customWidth="1"/>
+    <col min="7959" max="8192" width="9.125" style="237"/>
+    <col min="8193" max="8194" width="10" style="237" customWidth="1"/>
+    <col min="8195" max="8195" width="18" style="237" customWidth="1"/>
+    <col min="8196" max="8196" width="16" style="237" customWidth="1"/>
+    <col min="8197" max="8198" width="8.625" style="237" customWidth="1"/>
+    <col min="8199" max="8199" width="12.875" style="237" customWidth="1"/>
+    <col min="8200" max="8200" width="14.75" style="237" customWidth="1"/>
+    <col min="8201" max="8201" width="14.125" style="237" customWidth="1"/>
+    <col min="8202" max="8202" width="14.75" style="237" customWidth="1"/>
+    <col min="8203" max="8203" width="9.125" style="237"/>
+    <col min="8204" max="8214" width="0" style="237" hidden="1" customWidth="1"/>
+    <col min="8215" max="8448" width="9.125" style="237"/>
+    <col min="8449" max="8450" width="10" style="237" customWidth="1"/>
+    <col min="8451" max="8451" width="18" style="237" customWidth="1"/>
+    <col min="8452" max="8452" width="16" style="237" customWidth="1"/>
+    <col min="8453" max="8454" width="8.625" style="237" customWidth="1"/>
+    <col min="8455" max="8455" width="12.875" style="237" customWidth="1"/>
+    <col min="8456" max="8456" width="14.75" style="237" customWidth="1"/>
+    <col min="8457" max="8457" width="14.125" style="237" customWidth="1"/>
+    <col min="8458" max="8458" width="14.75" style="237" customWidth="1"/>
+    <col min="8459" max="8459" width="9.125" style="237"/>
+    <col min="8460" max="8470" width="0" style="237" hidden="1" customWidth="1"/>
+    <col min="8471" max="8704" width="9.125" style="237"/>
+    <col min="8705" max="8706" width="10" style="237" customWidth="1"/>
+    <col min="8707" max="8707" width="18" style="237" customWidth="1"/>
+    <col min="8708" max="8708" width="16" style="237" customWidth="1"/>
+    <col min="8709" max="8710" width="8.625" style="237" customWidth="1"/>
+    <col min="8711" max="8711" width="12.875" style="237" customWidth="1"/>
+    <col min="8712" max="8712" width="14.75" style="237" customWidth="1"/>
+    <col min="8713" max="8713" width="14.125" style="237" customWidth="1"/>
+    <col min="8714" max="8714" width="14.75" style="237" customWidth="1"/>
+    <col min="8715" max="8715" width="9.125" style="237"/>
+    <col min="8716" max="8726" width="0" style="237" hidden="1" customWidth="1"/>
+    <col min="8727" max="8960" width="9.125" style="237"/>
+    <col min="8961" max="8962" width="10" style="237" customWidth="1"/>
+    <col min="8963" max="8963" width="18" style="237" customWidth="1"/>
+    <col min="8964" max="8964" width="16" style="237" customWidth="1"/>
+    <col min="8965" max="8966" width="8.625" style="237" customWidth="1"/>
+    <col min="8967" max="8967" width="12.875" style="237" customWidth="1"/>
+    <col min="8968" max="8968" width="14.75" style="237" customWidth="1"/>
+    <col min="8969" max="8969" width="14.125" style="237" customWidth="1"/>
+    <col min="8970" max="8970" width="14.75" style="237" customWidth="1"/>
+    <col min="8971" max="8971" width="9.125" style="237"/>
+    <col min="8972" max="8982" width="0" style="237" hidden="1" customWidth="1"/>
+    <col min="8983" max="9216" width="9.125" style="237"/>
+    <col min="9217" max="9218" width="10" style="237" customWidth="1"/>
+    <col min="9219" max="9219" width="18" style="237" customWidth="1"/>
+    <col min="9220" max="9220" width="16" style="237" customWidth="1"/>
+    <col min="9221" max="9222" width="8.625" style="237" customWidth="1"/>
+    <col min="9223" max="9223" width="12.875" style="237" customWidth="1"/>
+    <col min="9224" max="9224" width="14.75" style="237" customWidth="1"/>
+    <col min="9225" max="9225" width="14.125" style="237" customWidth="1"/>
+    <col min="9226" max="9226" width="14.75" style="237" customWidth="1"/>
+    <col min="9227" max="9227" width="9.125" style="237"/>
+    <col min="9228" max="9238" width="0" style="237" hidden="1" customWidth="1"/>
+    <col min="9239" max="9472" width="9.125" style="237"/>
+    <col min="9473" max="9474" width="10" style="237" customWidth="1"/>
+    <col min="9475" max="9475" width="18" style="237" customWidth="1"/>
+    <col min="9476" max="9476" width="16" style="237" customWidth="1"/>
+    <col min="9477" max="9478" width="8.625" style="237" customWidth="1"/>
+    <col min="9479" max="9479" width="12.875" style="237" customWidth="1"/>
+    <col min="9480" max="9480" width="14.75" style="237" customWidth="1"/>
+    <col min="9481" max="9481" width="14.125" style="237" customWidth="1"/>
+    <col min="9482" max="9482" width="14.75" style="237" customWidth="1"/>
+    <col min="9483" max="9483" width="9.125" style="237"/>
+    <col min="9484" max="9494" width="0" style="237" hidden="1" customWidth="1"/>
+    <col min="9495" max="9728" width="9.125" style="237"/>
+    <col min="9729" max="9730" width="10" style="237" customWidth="1"/>
+    <col min="9731" max="9731" width="18" style="237" customWidth="1"/>
+    <col min="9732" max="9732" width="16" style="237" customWidth="1"/>
+    <col min="9733" max="9734" width="8.625" style="237" customWidth="1"/>
+    <col min="9735" max="9735" width="12.875" style="237" customWidth="1"/>
+    <col min="9736" max="9736" width="14.75" style="237" customWidth="1"/>
+    <col min="9737" max="9737" width="14.125" style="237" customWidth="1"/>
+    <col min="9738" max="9738" width="14.75" style="237" customWidth="1"/>
+    <col min="9739" max="9739" width="9.125" style="237"/>
+    <col min="9740" max="9750" width="0" style="237" hidden="1" customWidth="1"/>
+    <col min="9751" max="9984" width="9.125" style="237"/>
+    <col min="9985" max="9986" width="10" style="237" customWidth="1"/>
+    <col min="9987" max="9987" width="18" style="237" customWidth="1"/>
+    <col min="9988" max="9988" width="16" style="237" customWidth="1"/>
+    <col min="9989" max="9990" width="8.625" style="237" customWidth="1"/>
+    <col min="9991" max="9991" width="12.875" style="237" customWidth="1"/>
+    <col min="9992" max="9992" width="14.75" style="237" customWidth="1"/>
+    <col min="9993" max="9993" width="14.125" style="237" customWidth="1"/>
+    <col min="9994" max="9994" width="14.75" style="237" customWidth="1"/>
+    <col min="9995" max="9995" width="9.125" style="237"/>
+    <col min="9996" max="10006" width="0" style="237" hidden="1" customWidth="1"/>
+    <col min="10007" max="10240" width="9.125" style="237"/>
+    <col min="10241" max="10242" width="10" style="237" customWidth="1"/>
+    <col min="10243" max="10243" width="18" style="237" customWidth="1"/>
+    <col min="10244" max="10244" width="16" style="237" customWidth="1"/>
+    <col min="10245" max="10246" width="8.625" style="237" customWidth="1"/>
+    <col min="10247" max="10247" width="12.875" style="237" customWidth="1"/>
+    <col min="10248" max="10248" width="14.75" style="237" customWidth="1"/>
+    <col min="10249" max="10249" width="14.125" style="237" customWidth="1"/>
+    <col min="10250" max="10250" width="14.75" style="237" customWidth="1"/>
+    <col min="10251" max="10251" width="9.125" style="237"/>
+    <col min="10252" max="10262" width="0" style="237" hidden="1" customWidth="1"/>
+    <col min="10263" max="10496" width="9.125" style="237"/>
+    <col min="10497" max="10498" width="10" style="237" customWidth="1"/>
+    <col min="10499" max="10499" width="18" style="237" customWidth="1"/>
+    <col min="10500" max="10500" width="16" style="237" customWidth="1"/>
+    <col min="10501" max="10502" width="8.625" style="237" customWidth="1"/>
+    <col min="10503" max="10503" width="12.875" style="237" customWidth="1"/>
+    <col min="10504" max="10504" width="14.75" style="237" customWidth="1"/>
+    <col min="10505" max="10505" width="14.125" style="237" customWidth="1"/>
+    <col min="10506" max="10506" width="14.75" style="237" customWidth="1"/>
+    <col min="10507" max="10507" width="9.125" style="237"/>
+    <col min="10508" max="10518" width="0" style="237" hidden="1" customWidth="1"/>
+    <col min="10519" max="10752" width="9.125" style="237"/>
+    <col min="10753" max="10754" width="10" style="237" customWidth="1"/>
+    <col min="10755" max="10755" width="18" style="237" customWidth="1"/>
+    <col min="10756" max="10756" width="16" style="237" customWidth="1"/>
+    <col min="10757" max="10758" width="8.625" style="237" customWidth="1"/>
+    <col min="10759" max="10759" width="12.875" style="237" customWidth="1"/>
+    <col min="10760" max="10760" width="14.75" style="237" customWidth="1"/>
+    <col min="10761" max="10761" width="14.125" style="237" customWidth="1"/>
+    <col min="10762" max="10762" width="14.75" style="237" customWidth="1"/>
+    <col min="10763" max="10763" width="9.125" style="237"/>
+    <col min="10764" max="10774" width="0" style="237" hidden="1" customWidth="1"/>
+    <col min="10775" max="11008" width="9.125" style="237"/>
+    <col min="11009" max="11010" width="10" style="237" customWidth="1"/>
+    <col min="11011" max="11011" width="18" style="237" customWidth="1"/>
+    <col min="11012" max="11012" width="16" style="237" customWidth="1"/>
+    <col min="11013" max="11014" width="8.625" style="237" customWidth="1"/>
+    <col min="11015" max="11015" width="12.875" style="237" customWidth="1"/>
+    <col min="11016" max="11016" width="14.75" style="237" customWidth="1"/>
+    <col min="11017" max="11017" width="14.125" style="237" customWidth="1"/>
+    <col min="11018" max="11018" width="14.75" style="237" customWidth="1"/>
+    <col min="11019" max="11019" width="9.125" style="237"/>
+    <col min="11020" max="11030" width="0" style="237" hidden="1" customWidth="1"/>
+    <col min="11031" max="11264" width="9.125" style="237"/>
+    <col min="11265" max="11266" width="10" style="237" customWidth="1"/>
+    <col min="11267" max="11267" width="18" style="237" customWidth="1"/>
+    <col min="11268" max="11268" width="16" style="237" customWidth="1"/>
+    <col min="11269" max="11270" width="8.625" style="237" customWidth="1"/>
+    <col min="11271" max="11271" width="12.875" style="237" customWidth="1"/>
+    <col min="11272" max="11272" width="14.75" style="237" customWidth="1"/>
+    <col min="11273" max="11273" width="14.125" style="237" customWidth="1"/>
+    <col min="11274" max="11274" width="14.75" style="237" customWidth="1"/>
+    <col min="11275" max="11275" width="9.125" style="237"/>
+    <col min="11276" max="11286" width="0" style="237" hidden="1" customWidth="1"/>
+    <col min="11287" max="11520" width="9.125" style="237"/>
+    <col min="11521" max="11522" width="10" style="237" customWidth="1"/>
+    <col min="11523" max="11523" width="18" style="237" customWidth="1"/>
+    <col min="11524" max="11524" width="16" style="237" customWidth="1"/>
+    <col min="11525" max="11526" width="8.625" style="237" customWidth="1"/>
+    <col min="11527" max="11527" width="12.875" style="237" customWidth="1"/>
+    <col min="11528" max="11528" width="14.75" style="237" customWidth="1"/>
+    <col min="11529" max="11529" width="14.125" style="237" customWidth="1"/>
+    <col min="11530" max="11530" width="14.75" style="237" customWidth="1"/>
+    <col min="11531" max="11531" width="9.125" style="237"/>
+    <col min="11532" max="11542" width="0" style="237" hidden="1" customWidth="1"/>
+    <col min="11543" max="11776" width="9.125" style="237"/>
+    <col min="11777" max="11778" width="10" style="237" customWidth="1"/>
+    <col min="11779" max="11779" width="18" style="237" customWidth="1"/>
+    <col min="11780" max="11780" width="16" style="237" customWidth="1"/>
+    <col min="11781" max="11782" width="8.625" style="237" customWidth="1"/>
+    <col min="11783" max="11783" width="12.875" style="237" customWidth="1"/>
+    <col min="11784" max="11784" width="14.75" style="237" customWidth="1"/>
+    <col min="11785" max="11785" width="14.125" style="237" customWidth="1"/>
+    <col min="11786" max="11786" width="14.75" style="237" customWidth="1"/>
+    <col min="11787" max="11787" width="9.125" style="237"/>
+    <col min="11788" max="11798" width="0" style="237" hidden="1" customWidth="1"/>
+    <col min="11799" max="12032" width="9.125" style="237"/>
+    <col min="12033" max="12034" width="10" style="237" customWidth="1"/>
+    <col min="12035" max="12035" width="18" style="237" customWidth="1"/>
+    <col min="12036" max="12036" width="16" style="237" customWidth="1"/>
+    <col min="12037" max="12038" width="8.625" style="237" customWidth="1"/>
+    <col min="12039" max="12039" width="12.875" style="237" customWidth="1"/>
+    <col min="12040" max="12040" width="14.75" style="237" customWidth="1"/>
+    <col min="12041" max="12041" width="14.125" style="237" customWidth="1"/>
+    <col min="12042" max="12042" width="14.75" style="237" customWidth="1"/>
+    <col min="12043" max="12043" width="9.125" style="237"/>
+    <col min="12044" max="12054" width="0" style="237" hidden="1" customWidth="1"/>
+    <col min="12055" max="12288" width="9.125" style="237"/>
+    <col min="12289" max="12290" width="10" style="237" customWidth="1"/>
+    <col min="12291" max="12291" width="18" style="237" customWidth="1"/>
+    <col min="12292" max="12292" width="16" style="237" customWidth="1"/>
+    <col min="12293" max="12294" width="8.625" style="237" customWidth="1"/>
+    <col min="12295" max="12295" width="12.875" style="237" customWidth="1"/>
+    <col min="12296" max="12296" width="14.75" style="237" customWidth="1"/>
+    <col min="12297" max="12297" width="14.125" style="237" customWidth="1"/>
+    <col min="12298" max="12298" width="14.75" style="237" customWidth="1"/>
+    <col min="12299" max="12299" width="9.125" style="237"/>
+    <col min="12300" max="12310" width="0" style="237" hidden="1" customWidth="1"/>
+    <col min="12311" max="12544" width="9.125" style="237"/>
+    <col min="12545" max="12546" width="10" style="237" customWidth="1"/>
+    <col min="12547" max="12547" width="18" style="237" customWidth="1"/>
+    <col min="12548" max="12548" width="16" style="237" customWidth="1"/>
+    <col min="12549" max="12550" width="8.625" style="237" customWidth="1"/>
+    <col min="12551" max="12551" width="12.875" style="237" customWidth="1"/>
+    <col min="12552" max="12552" width="14.75" style="237" customWidth="1"/>
+    <col min="12553" max="12553" width="14.125" style="237" customWidth="1"/>
+    <col min="12554" max="12554" width="14.75" style="237" customWidth="1"/>
+    <col min="12555" max="12555" width="9.125" style="237"/>
+    <col min="12556" max="12566" width="0" style="237" hidden="1" customWidth="1"/>
+    <col min="12567" max="12800" width="9.125" style="237"/>
+    <col min="12801" max="12802" width="10" style="237" customWidth="1"/>
+    <col min="12803" max="12803" width="18" style="237" customWidth="1"/>
+    <col min="12804" max="12804" width="16" style="237" customWidth="1"/>
+    <col min="12805" max="12806" width="8.625" style="237" customWidth="1"/>
+    <col min="12807" max="12807" width="12.875" style="237" customWidth="1"/>
+    <col min="12808" max="12808" width="14.75" style="237" customWidth="1"/>
+    <col min="12809" max="12809" width="14.125" style="237" customWidth="1"/>
+    <col min="12810" max="12810" width="14.75" style="237" customWidth="1"/>
+    <col min="12811" max="12811" width="9.125" style="237"/>
+    <col min="12812" max="12822" width="0" style="237" hidden="1" customWidth="1"/>
+    <col min="12823" max="13056" width="9.125" style="237"/>
+    <col min="13057" max="13058" width="10" style="237" customWidth="1"/>
+    <col min="13059" max="13059" width="18" style="237" customWidth="1"/>
+    <col min="13060" max="13060" width="16" style="237" customWidth="1"/>
+    <col min="13061" max="13062" width="8.625" style="237" customWidth="1"/>
+    <col min="13063" max="13063" width="12.875" style="237" customWidth="1"/>
+    <col min="13064" max="13064" width="14.75" style="237" customWidth="1"/>
+    <col min="13065" max="13065" width="14.125" style="237" customWidth="1"/>
+    <col min="13066" max="13066" width="14.75" style="237" customWidth="1"/>
+    <col min="13067" max="13067" width="9.125" style="237"/>
+    <col min="13068" max="13078" width="0" style="237" hidden="1" customWidth="1"/>
+    <col min="13079" max="13312" width="9.125" style="237"/>
+    <col min="13313" max="13314" width="10" style="237" customWidth="1"/>
+    <col min="13315" max="13315" width="18" style="237" customWidth="1"/>
+    <col min="13316" max="13316" width="16" style="237" customWidth="1"/>
+    <col min="13317" max="13318" width="8.625" style="237" customWidth="1"/>
+    <col min="13319" max="13319" width="12.875" style="237" customWidth="1"/>
+    <col min="13320" max="13320" width="14.75" style="237" customWidth="1"/>
+    <col min="13321" max="13321" width="14.125" style="237" customWidth="1"/>
+    <col min="13322" max="13322" width="14.75" style="237" customWidth="1"/>
+    <col min="13323" max="13323" width="9.125" style="237"/>
+    <col min="13324" max="13334" width="0" style="237" hidden="1" customWidth="1"/>
+    <col min="13335" max="13568" width="9.125" style="237"/>
+    <col min="13569" max="13570" width="10" style="237" customWidth="1"/>
+    <col min="13571" max="13571" width="18" style="237" customWidth="1"/>
+    <col min="13572" max="13572" width="16" style="237" customWidth="1"/>
+    <col min="13573" max="13574" width="8.625" style="237" customWidth="1"/>
+    <col min="13575" max="13575" width="12.875" style="237" customWidth="1"/>
+    <col min="13576" max="13576" width="14.75" style="237" customWidth="1"/>
+    <col min="13577" max="13577" width="14.125" style="237" customWidth="1"/>
+    <col min="13578" max="13578" width="14.75" style="237" customWidth="1"/>
+    <col min="13579" max="13579" width="9.125" style="237"/>
+    <col min="13580" max="13590" width="0" style="237" hidden="1" customWidth="1"/>
+    <col min="13591" max="13824" width="9.125" style="237"/>
+    <col min="13825" max="13826" width="10" style="237" customWidth="1"/>
+    <col min="13827" max="13827" width="18" style="237" customWidth="1"/>
+    <col min="13828" max="13828" width="16" style="237" customWidth="1"/>
+    <col min="13829" max="13830" width="8.625" style="237" customWidth="1"/>
+    <col min="13831" max="13831" width="12.875" style="237" customWidth="1"/>
+    <col min="13832" max="13832" width="14.75" style="237" customWidth="1"/>
+    <col min="13833" max="13833" width="14.125" style="237" customWidth="1"/>
+    <col min="13834" max="13834" width="14.75" style="237" customWidth="1"/>
+    <col min="13835" max="13835" width="9.125" style="237"/>
+    <col min="13836" max="13846" width="0" style="237" hidden="1" customWidth="1"/>
+    <col min="13847" max="14080" width="9.125" style="237"/>
+    <col min="14081" max="14082" width="10" style="237" customWidth="1"/>
+    <col min="14083" max="14083" width="18" style="237" customWidth="1"/>
+    <col min="14084" max="14084" width="16" style="237" customWidth="1"/>
+    <col min="14085" max="14086" width="8.625" style="237" customWidth="1"/>
+    <col min="14087" max="14087" width="12.875" style="237" customWidth="1"/>
+    <col min="14088" max="14088" width="14.75" style="237" customWidth="1"/>
+    <col min="14089" max="14089" width="14.125" style="237" customWidth="1"/>
+    <col min="14090" max="14090" width="14.75" style="237" customWidth="1"/>
+    <col min="14091" max="14091" width="9.125" style="237"/>
+    <col min="14092" max="14102" width="0" style="237" hidden="1" customWidth="1"/>
+    <col min="14103" max="14336" width="9.125" style="237"/>
+    <col min="14337" max="14338" width="10" style="237" customWidth="1"/>
+    <col min="14339" max="14339" width="18" style="237" customWidth="1"/>
+    <col min="14340" max="14340" width="16" style="237" customWidth="1"/>
+    <col min="14341" max="14342" width="8.625" style="237" customWidth="1"/>
+    <col min="14343" max="14343" width="12.875" style="237" customWidth="1"/>
+    <col min="14344" max="14344" width="14.75" style="237" customWidth="1"/>
+    <col min="14345" max="14345" width="14.125" style="237" customWidth="1"/>
+    <col min="14346" max="14346" width="14.75" style="237" customWidth="1"/>
+    <col min="14347" max="14347" width="9.125" style="237"/>
+    <col min="14348" max="14358" width="0" style="237" hidden="1" customWidth="1"/>
+    <col min="14359" max="14592" width="9.125" style="237"/>
+    <col min="14593" max="14594" width="10" style="237" customWidth="1"/>
+    <col min="14595" max="14595" width="18" style="237" customWidth="1"/>
+    <col min="14596" max="14596" width="16" style="237" customWidth="1"/>
+    <col min="14597" max="14598" width="8.625" style="237" customWidth="1"/>
+    <col min="14599" max="14599" width="12.875" style="237" customWidth="1"/>
+    <col min="14600" max="14600" width="14.75" style="237" customWidth="1"/>
+    <col min="14601" max="14601" width="14.125" style="237" customWidth="1"/>
+    <col min="14602" max="14602" width="14.75" style="237" customWidth="1"/>
+    <col min="14603" max="14603" width="9.125" style="237"/>
+    <col min="14604" max="14614" width="0" style="237" hidden="1" customWidth="1"/>
+    <col min="14615" max="14848" width="9.125" style="237"/>
+    <col min="14849" max="14850" width="10" style="237" customWidth="1"/>
+    <col min="14851" max="14851" width="18" style="237" customWidth="1"/>
+    <col min="14852" max="14852" width="16" style="237" customWidth="1"/>
+    <col min="14853" max="14854" width="8.625" style="237" customWidth="1"/>
+    <col min="14855" max="14855" width="12.875" style="237" customWidth="1"/>
+    <col min="14856" max="14856" width="14.75" style="237" customWidth="1"/>
+    <col min="14857" max="14857" width="14.125" style="237" customWidth="1"/>
+    <col min="14858" max="14858" width="14.75" style="237" customWidth="1"/>
+    <col min="14859" max="14859" width="9.125" style="237"/>
+    <col min="14860" max="14870" width="0" style="237" hidden="1" customWidth="1"/>
+    <col min="14871" max="15104" width="9.125" style="237"/>
+    <col min="15105" max="15106" width="10" style="237" customWidth="1"/>
+    <col min="15107" max="15107" width="18" style="237" customWidth="1"/>
+    <col min="15108" max="15108" width="16" style="237" customWidth="1"/>
+    <col min="15109" max="15110" width="8.625" style="237" customWidth="1"/>
+    <col min="15111" max="15111" width="12.875" style="237" customWidth="1"/>
+    <col min="15112" max="15112" width="14.75" style="237" customWidth="1"/>
+    <col min="15113" max="15113" width="14.125" style="237" customWidth="1"/>
+    <col min="15114" max="15114" width="14.75" style="237" customWidth="1"/>
+    <col min="15115" max="15115" width="9.125" style="237"/>
+    <col min="15116" max="15126" width="0" style="237" hidden="1" customWidth="1"/>
+    <col min="15127" max="15360" width="9.125" style="237"/>
+    <col min="15361" max="15362" width="10" style="237" customWidth="1"/>
+    <col min="15363" max="15363" width="18" style="237" customWidth="1"/>
+    <col min="15364" max="15364" width="16" style="237" customWidth="1"/>
+    <col min="15365" max="15366" width="8.625" style="237" customWidth="1"/>
+    <col min="15367" max="15367" width="12.875" style="237" customWidth="1"/>
+    <col min="15368" max="15368" width="14.75" style="237" customWidth="1"/>
+    <col min="15369" max="15369" width="14.125" style="237" customWidth="1"/>
+    <col min="15370" max="15370" width="14.75" style="237" customWidth="1"/>
+    <col min="15371" max="15371" width="9.125" style="237"/>
+    <col min="15372" max="15382" width="0" style="237" hidden="1" customWidth="1"/>
+    <col min="15383" max="15616" width="9.125" style="237"/>
+    <col min="15617" max="15618" width="10" style="237" customWidth="1"/>
+    <col min="15619" max="15619" width="18" style="237" customWidth="1"/>
+    <col min="15620" max="15620" width="16" style="237" customWidth="1"/>
+    <col min="15621" max="15622" width="8.625" style="237" customWidth="1"/>
+    <col min="15623" max="15623" width="12.875" style="237" customWidth="1"/>
+    <col min="15624" max="15624" width="14.75" style="237" customWidth="1"/>
+    <col min="15625" max="15625" width="14.125" style="237" customWidth="1"/>
+    <col min="15626" max="15626" width="14.75" style="237" customWidth="1"/>
+    <col min="15627" max="15627" width="9.125" style="237"/>
+    <col min="15628" max="15638" width="0" style="237" hidden="1" customWidth="1"/>
+    <col min="15639" max="15872" width="9.125" style="237"/>
+    <col min="15873" max="15874" width="10" style="237" customWidth="1"/>
+    <col min="15875" max="15875" width="18" style="237" customWidth="1"/>
+    <col min="15876" max="15876" width="16" style="237" customWidth="1"/>
+    <col min="15877" max="15878" width="8.625" style="237" customWidth="1"/>
+    <col min="15879" max="15879" width="12.875" style="237" customWidth="1"/>
+    <col min="15880" max="15880" width="14.75" style="237" customWidth="1"/>
+    <col min="15881" max="15881" width="14.125" style="237" customWidth="1"/>
+    <col min="15882" max="15882" width="14.75" style="237" customWidth="1"/>
+    <col min="15883" max="15883" width="9.125" style="237"/>
+    <col min="15884" max="15894" width="0" style="237" hidden="1" customWidth="1"/>
+    <col min="15895" max="16128" width="9.125" style="237"/>
+    <col min="16129" max="16130" width="10" style="237" customWidth="1"/>
+    <col min="16131" max="16131" width="18" style="237" customWidth="1"/>
+    <col min="16132" max="16132" width="16" style="237" customWidth="1"/>
+    <col min="16133" max="16134" width="8.625" style="237" customWidth="1"/>
+    <col min="16135" max="16135" width="12.875" style="237" customWidth="1"/>
+    <col min="16136" max="16136" width="14.75" style="237" customWidth="1"/>
+    <col min="16137" max="16137" width="14.125" style="237" customWidth="1"/>
+    <col min="16138" max="16138" width="14.75" style="237" customWidth="1"/>
+    <col min="16139" max="16139" width="9.125" style="237"/>
+    <col min="16140" max="16150" width="0" style="237" hidden="1" customWidth="1"/>
+    <col min="16151" max="16384" width="9.125" style="237"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="74" customFormat="1" ht="27.75" customHeight="1" thickBot="1">
@@ -4955,8 +4949,8 @@
         <v>1</v>
       </c>
       <c r="H1" s="73"/>
-      <c r="I1" s="284"/>
-      <c r="J1" s="285"/>
+      <c r="I1" s="276"/>
+      <c r="J1" s="277"/>
       <c r="L1" s="1" t="s">
         <v>2</v>
       </c>
@@ -4987,10 +4981,10 @@
       <c r="H2" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="270" t="s">
+      <c r="I2" s="278" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="271"/>
+      <c r="J2" s="279"/>
       <c r="L2" s="5"/>
       <c r="M2" s="6"/>
       <c r="N2" s="6"/>
@@ -5012,13 +5006,13 @@
         <v>10</v>
       </c>
       <c r="E3" s="85"/>
-      <c r="F3" s="286" t="s">
+      <c r="F3" s="280" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="287"/>
+      <c r="G3" s="281"/>
       <c r="H3" s="88"/>
-      <c r="I3" s="288"/>
-      <c r="J3" s="289"/>
+      <c r="I3" s="282"/>
+      <c r="J3" s="283"/>
       <c r="L3" s="8" t="s">
         <v>12</v>
       </c>
@@ -5034,17 +5028,17 @@
       <c r="A4" s="89" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="292"/>
-      <c r="C4" s="293"/>
+      <c r="B4" s="286"/>
+      <c r="C4" s="287"/>
       <c r="D4" s="90" t="s">
         <v>152</v>
       </c>
       <c r="E4" s="91"/>
       <c r="F4" s="92"/>
-      <c r="G4" s="239"/>
+      <c r="G4" s="238"/>
       <c r="H4" s="93"/>
-      <c r="I4" s="290"/>
-      <c r="J4" s="291"/>
+      <c r="I4" s="284"/>
+      <c r="J4" s="285"/>
       <c r="L4" s="94" t="s">
         <v>15</v>
       </c>
@@ -5234,16 +5228,16 @@
     </row>
     <row r="9" spans="1:19" s="129" customFormat="1" ht="25.2" thickTop="1">
       <c r="A9" s="125"/>
-      <c r="B9" s="240"/>
-      <c r="C9" s="241"/>
-      <c r="D9" s="242"/>
-      <c r="E9" s="243"/>
-      <c r="F9" s="244"/>
-      <c r="G9" s="297">
+      <c r="B9" s="239"/>
+      <c r="C9" s="240"/>
+      <c r="D9" s="241"/>
+      <c r="E9" s="242"/>
+      <c r="F9" s="243"/>
+      <c r="G9" s="258">
         <f>E9*G4/1000</f>
         <v>0</v>
       </c>
-      <c r="H9" s="298"/>
+      <c r="H9" s="259"/>
       <c r="I9" s="127" t="s">
         <v>53</v>
       </c>
@@ -5273,16 +5267,16 @@
     </row>
     <row r="10" spans="1:19" s="129" customFormat="1" ht="24.6">
       <c r="A10" s="125"/>
-      <c r="B10" s="245"/>
-      <c r="C10" s="246"/>
-      <c r="D10" s="247"/>
-      <c r="E10" s="248"/>
-      <c r="F10" s="249"/>
-      <c r="G10" s="299">
+      <c r="B10" s="244"/>
+      <c r="C10" s="245"/>
+      <c r="D10" s="246"/>
+      <c r="E10" s="247"/>
+      <c r="F10" s="248"/>
+      <c r="G10" s="260">
         <f>E10*G4/1000</f>
         <v>0</v>
       </c>
-      <c r="H10" s="300"/>
+      <c r="H10" s="261"/>
       <c r="I10" s="127" t="s">
         <v>56</v>
       </c>
@@ -5302,16 +5296,16 @@
       <c r="A11" s="125" t="s">
         <v>58</v>
       </c>
-      <c r="B11" s="245"/>
-      <c r="C11" s="246"/>
-      <c r="D11" s="247"/>
-      <c r="E11" s="248"/>
-      <c r="F11" s="249"/>
-      <c r="G11" s="301">
+      <c r="B11" s="244"/>
+      <c r="C11" s="245"/>
+      <c r="D11" s="246"/>
+      <c r="E11" s="247"/>
+      <c r="F11" s="248"/>
+      <c r="G11" s="262">
         <f>E11*G4/1000</f>
         <v>0</v>
       </c>
-      <c r="H11" s="300"/>
+      <c r="H11" s="261"/>
       <c r="I11" s="127" t="s">
         <v>59</v>
       </c>
@@ -5341,16 +5335,16 @@
     </row>
     <row r="12" spans="1:19" s="129" customFormat="1" ht="24.6">
       <c r="A12" s="131"/>
-      <c r="B12" s="245"/>
-      <c r="C12" s="246"/>
-      <c r="D12" s="247"/>
-      <c r="E12" s="248"/>
-      <c r="F12" s="249"/>
-      <c r="G12" s="301">
+      <c r="B12" s="244"/>
+      <c r="C12" s="245"/>
+      <c r="D12" s="246"/>
+      <c r="E12" s="247"/>
+      <c r="F12" s="248"/>
+      <c r="G12" s="262">
         <f>E12*G4/1000</f>
         <v>0</v>
       </c>
-      <c r="H12" s="300"/>
+      <c r="H12" s="261"/>
       <c r="I12" s="132" t="s">
         <v>62</v>
       </c>
@@ -5397,7 +5391,7 @@
         <f>SUM(G9:G12)</f>
         <v>0</v>
       </c>
-      <c r="H13" s="303"/>
+      <c r="H13" s="264"/>
       <c r="I13" s="136"/>
       <c r="J13" s="137"/>
       <c r="L13" s="34"/>
@@ -5673,16 +5667,16 @@
     </row>
     <row r="21" spans="1:19" s="83" customFormat="1" ht="25.2" thickTop="1">
       <c r="A21" s="125"/>
-      <c r="B21" s="250"/>
-      <c r="C21" s="241"/>
-      <c r="D21" s="242"/>
-      <c r="E21" s="251"/>
-      <c r="F21" s="244"/>
-      <c r="G21" s="297">
+      <c r="B21" s="249"/>
+      <c r="C21" s="240"/>
+      <c r="D21" s="241"/>
+      <c r="E21" s="250"/>
+      <c r="F21" s="243"/>
+      <c r="G21" s="258">
         <f>E21*G4/1000</f>
         <v>0</v>
       </c>
-      <c r="H21" s="304"/>
+      <c r="H21" s="265"/>
       <c r="I21" s="127" t="s">
         <v>82</v>
       </c>
@@ -5698,16 +5692,16 @@
     </row>
     <row r="22" spans="1:19" s="83" customFormat="1" ht="24.6">
       <c r="A22" s="125"/>
-      <c r="B22" s="245"/>
-      <c r="C22" s="246"/>
-      <c r="D22" s="252"/>
-      <c r="E22" s="248"/>
-      <c r="F22" s="253"/>
-      <c r="G22" s="301">
+      <c r="B22" s="244"/>
+      <c r="C22" s="245"/>
+      <c r="D22" s="251"/>
+      <c r="E22" s="247"/>
+      <c r="F22" s="252"/>
+      <c r="G22" s="262">
         <f>E22*G4/1000</f>
         <v>0</v>
       </c>
-      <c r="H22" s="305"/>
+      <c r="H22" s="266"/>
       <c r="I22" s="127" t="s">
         <v>83</v>
       </c>
@@ -5737,16 +5731,16 @@
       <c r="A23" s="125" t="s">
         <v>85</v>
       </c>
-      <c r="B23" s="245"/>
-      <c r="C23" s="246"/>
-      <c r="D23" s="252"/>
-      <c r="E23" s="254"/>
-      <c r="F23" s="255"/>
-      <c r="G23" s="301">
+      <c r="B23" s="244"/>
+      <c r="C23" s="245"/>
+      <c r="D23" s="251"/>
+      <c r="E23" s="253"/>
+      <c r="F23" s="254"/>
+      <c r="G23" s="262">
         <f>E23*G4/1000</f>
         <v>0</v>
       </c>
-      <c r="H23" s="305"/>
+      <c r="H23" s="266"/>
       <c r="I23" s="127" t="s">
         <v>86</v>
       </c>
@@ -5776,16 +5770,16 @@
       <c r="A24" s="125" t="s">
         <v>88</v>
       </c>
-      <c r="B24" s="245"/>
-      <c r="C24" s="246"/>
-      <c r="D24" s="247"/>
-      <c r="E24" s="248"/>
-      <c r="F24" s="253"/>
-      <c r="G24" s="301">
+      <c r="B24" s="244"/>
+      <c r="C24" s="245"/>
+      <c r="D24" s="246"/>
+      <c r="E24" s="247"/>
+      <c r="F24" s="252"/>
+      <c r="G24" s="262">
         <f>E24*G4/1000</f>
         <v>0</v>
       </c>
-      <c r="H24" s="305"/>
+      <c r="H24" s="266"/>
       <c r="I24" s="132" t="s">
         <v>62</v>
       </c>
@@ -5834,7 +5828,7 @@
         <f>SUM(G21:G24)</f>
         <v>0</v>
       </c>
-      <c r="H25" s="305"/>
+      <c r="H25" s="266"/>
       <c r="I25" s="164"/>
       <c r="J25" s="137"/>
       <c r="L25" s="20"/>
@@ -5983,12 +5977,12 @@
         <v>102</v>
       </c>
       <c r="F30" s="168"/>
-      <c r="G30" s="294" t="s">
+      <c r="G30" s="273" t="s">
         <v>103</v>
       </c>
-      <c r="H30" s="295"/>
-      <c r="I30" s="295"/>
-      <c r="J30" s="296"/>
+      <c r="H30" s="274"/>
+      <c r="I30" s="274"/>
+      <c r="J30" s="275"/>
       <c r="L30" s="50"/>
       <c r="M30" s="23" t="s">
         <v>104</v>
@@ -6017,10 +6011,10 @@
         <v>108</v>
       </c>
       <c r="F31" s="168"/>
-      <c r="G31" s="294"/>
-      <c r="H31" s="295"/>
-      <c r="I31" s="295"/>
-      <c r="J31" s="296"/>
+      <c r="G31" s="273"/>
+      <c r="H31" s="274"/>
+      <c r="I31" s="274"/>
+      <c r="J31" s="275"/>
       <c r="L31" s="50"/>
       <c r="M31" s="23"/>
       <c r="N31" s="2"/>
@@ -6047,8 +6041,8 @@
         <v>112</v>
       </c>
       <c r="H32" s="175"/>
-      <c r="I32" s="278"/>
-      <c r="J32" s="279"/>
+      <c r="I32" s="288"/>
+      <c r="J32" s="289"/>
       <c r="L32" s="51" t="s">
         <v>113</v>
       </c>
@@ -6083,8 +6077,8 @@
         <v>118</v>
       </c>
       <c r="H33" s="179"/>
-      <c r="I33" s="280"/>
-      <c r="J33" s="281"/>
+      <c r="I33" s="290"/>
+      <c r="J33" s="291"/>
       <c r="L33" s="54"/>
       <c r="M33" s="55"/>
       <c r="N33" s="56"/>
@@ -6111,8 +6105,8 @@
         <v>121</v>
       </c>
       <c r="H34" s="183"/>
-      <c r="I34" s="282"/>
-      <c r="J34" s="283"/>
+      <c r="I34" s="292"/>
+      <c r="J34" s="293"/>
       <c r="L34" s="54"/>
       <c r="M34" s="55"/>
       <c r="N34" s="56"/>
@@ -6123,7 +6117,7 @@
       <c r="S34" s="59"/>
     </row>
     <row r="35" spans="1:19" s="83" customFormat="1" ht="24" thickTop="1">
-      <c r="A35" s="259" t="s">
+      <c r="A35" s="294" t="s">
         <v>122</v>
       </c>
       <c r="B35" s="171" t="s">
@@ -6141,8 +6135,8 @@
         <v>112</v>
       </c>
       <c r="H35" s="175"/>
-      <c r="I35" s="278"/>
-      <c r="J35" s="279"/>
+      <c r="I35" s="288"/>
+      <c r="J35" s="289"/>
       <c r="L35" s="54"/>
       <c r="M35" s="55"/>
       <c r="N35" s="56"/>
@@ -6153,7 +6147,7 @@
       <c r="S35" s="59"/>
     </row>
     <row r="36" spans="1:19" s="83" customFormat="1" ht="23.4">
-      <c r="A36" s="260"/>
+      <c r="A36" s="295"/>
       <c r="B36" s="143" t="s">
         <v>116</v>
       </c>
@@ -6169,8 +6163,8 @@
         <v>118</v>
       </c>
       <c r="H36" s="179"/>
-      <c r="I36" s="280"/>
-      <c r="J36" s="281"/>
+      <c r="I36" s="290"/>
+      <c r="J36" s="291"/>
       <c r="L36" s="60"/>
       <c r="M36" s="61"/>
       <c r="N36" s="61"/>
@@ -6187,7 +6181,7 @@
       </c>
     </row>
     <row r="37" spans="1:19" s="83" customFormat="1" ht="24" thickBot="1">
-      <c r="A37" s="261"/>
+      <c r="A37" s="296"/>
       <c r="B37" s="119" t="s">
         <v>119</v>
       </c>
@@ -6203,18 +6197,18 @@
         <v>121</v>
       </c>
       <c r="H37" s="183"/>
-      <c r="I37" s="282"/>
-      <c r="J37" s="283"/>
+      <c r="I37" s="292"/>
+      <c r="J37" s="293"/>
       <c r="Q37" s="28"/>
       <c r="R37" s="63"/>
       <c r="S37" s="63"/>
     </row>
     <row r="38" spans="1:19" s="83" customFormat="1" ht="21" thickTop="1">
-      <c r="A38" s="262" t="s">
+      <c r="A38" s="297" t="s">
         <v>129</v>
       </c>
-      <c r="B38" s="263"/>
-      <c r="C38" s="263"/>
+      <c r="B38" s="298"/>
+      <c r="C38" s="298"/>
       <c r="D38" s="184"/>
       <c r="E38" s="185" t="s">
         <v>130</v>
@@ -6233,9 +6227,9 @@
       <c r="S38" s="37"/>
     </row>
     <row r="39" spans="1:19" s="83" customFormat="1" ht="21" thickBot="1">
-      <c r="A39" s="264"/>
-      <c r="B39" s="265"/>
-      <c r="C39" s="265"/>
+      <c r="A39" s="299"/>
+      <c r="B39" s="300"/>
+      <c r="C39" s="300"/>
       <c r="D39" s="189"/>
       <c r="E39" s="190" t="s">
         <v>133</v>
@@ -6266,10 +6260,10 @@
       <c r="F40" s="195"/>
       <c r="G40" s="195"/>
       <c r="H40" s="195"/>
-      <c r="I40" s="268" t="s">
+      <c r="I40" s="303" t="s">
         <v>136</v>
       </c>
-      <c r="J40" s="269"/>
+      <c r="J40" s="304"/>
       <c r="L40" s="60"/>
       <c r="M40" s="61"/>
       <c r="N40" s="61"/>
@@ -6312,11 +6306,11 @@
         <v>137</v>
       </c>
       <c r="H42" s="197"/>
-      <c r="I42" s="284">
+      <c r="I42" s="276">
         <f>I1</f>
         <v>0</v>
       </c>
-      <c r="J42" s="285"/>
+      <c r="J42" s="277"/>
       <c r="L42" s="1"/>
       <c r="M42" s="1"/>
       <c r="N42" s="2"/>
@@ -6342,10 +6336,10 @@
       <c r="H43" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="I43" s="270" t="s">
+      <c r="I43" s="278" t="s">
         <v>8</v>
       </c>
-      <c r="J43" s="271"/>
+      <c r="J43" s="279"/>
       <c r="L43" s="1"/>
       <c r="M43" s="1"/>
       <c r="N43" s="66"/>
@@ -6367,11 +6361,11 @@
       </c>
       <c r="G44" s="200"/>
       <c r="H44" s="88"/>
-      <c r="I44" s="288">
+      <c r="I44" s="282">
         <f>I3</f>
         <v>0</v>
       </c>
-      <c r="J44" s="289"/>
+      <c r="J44" s="283"/>
       <c r="L44" s="1"/>
       <c r="M44" s="1"/>
       <c r="N44" s="2"/>
@@ -6385,23 +6379,23 @@
       <c r="A45" s="201" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="312">
+      <c r="B45" s="286">
         <f>B4</f>
         <v>0</v>
       </c>
-      <c r="C45" s="202"/>
-      <c r="D45" s="203" t="s">
+      <c r="C45" s="287"/>
+      <c r="D45" s="202" t="s">
         <v>14</v>
       </c>
-      <c r="E45" s="204"/>
-      <c r="F45" s="205"/>
-      <c r="G45" s="311">
+      <c r="E45" s="203"/>
+      <c r="F45" s="204"/>
+      <c r="G45" s="272">
         <f>G4</f>
         <v>0</v>
       </c>
       <c r="H45" s="88"/>
-      <c r="I45" s="288"/>
-      <c r="J45" s="289"/>
+      <c r="I45" s="282"/>
+      <c r="J45" s="283"/>
       <c r="L45" s="1"/>
       <c r="M45" s="1"/>
       <c r="N45" s="2"/>
@@ -6466,7 +6460,7 @@
       <c r="D48" s="110" t="s">
         <v>33</v>
       </c>
-      <c r="E48" s="206" t="s">
+      <c r="E48" s="205" t="s">
         <v>34</v>
       </c>
       <c r="F48" s="112"/>
@@ -6529,16 +6523,16 @@
     </row>
     <row r="50" spans="1:19" s="129" customFormat="1" ht="25.2" thickTop="1">
       <c r="A50" s="125"/>
-      <c r="B50" s="240"/>
-      <c r="C50" s="241"/>
-      <c r="D50" s="247"/>
-      <c r="E50" s="256"/>
-      <c r="F50" s="257"/>
-      <c r="G50" s="306">
+      <c r="B50" s="239"/>
+      <c r="C50" s="240"/>
+      <c r="D50" s="246"/>
+      <c r="E50" s="255"/>
+      <c r="F50" s="256"/>
+      <c r="G50" s="267">
         <f>G25</f>
         <v>0</v>
       </c>
-      <c r="H50" s="303"/>
+      <c r="H50" s="264"/>
       <c r="I50" s="127" t="s">
         <v>53</v>
       </c>
@@ -6548,16 +6542,16 @@
       <c r="A51" s="125" t="s">
         <v>140</v>
       </c>
-      <c r="B51" s="245"/>
-      <c r="C51" s="246"/>
-      <c r="D51" s="247"/>
-      <c r="E51" s="248"/>
-      <c r="F51" s="249"/>
-      <c r="G51" s="301">
+      <c r="B51" s="244"/>
+      <c r="C51" s="245"/>
+      <c r="D51" s="246"/>
+      <c r="E51" s="247"/>
+      <c r="F51" s="248"/>
+      <c r="G51" s="262">
         <f>E51*G4/1000</f>
         <v>0</v>
       </c>
-      <c r="H51" s="307"/>
+      <c r="H51" s="268"/>
       <c r="I51" s="127" t="s">
         <v>141</v>
       </c>
@@ -6575,21 +6569,21 @@
       <c r="A52" s="131" t="s">
         <v>88</v>
       </c>
-      <c r="B52" s="245"/>
-      <c r="C52" s="246"/>
-      <c r="D52" s="242"/>
-      <c r="E52" s="251"/>
-      <c r="F52" s="258"/>
-      <c r="G52" s="297">
+      <c r="B52" s="244"/>
+      <c r="C52" s="245"/>
+      <c r="D52" s="241"/>
+      <c r="E52" s="250"/>
+      <c r="F52" s="257"/>
+      <c r="G52" s="258">
         <f>E52*G45/1000</f>
         <v>0</v>
       </c>
-      <c r="H52" s="308"/>
+      <c r="H52" s="269"/>
       <c r="I52" s="127" t="s">
         <v>86</v>
       </c>
       <c r="J52" s="128"/>
-      <c r="L52" s="207"/>
+      <c r="L52" s="206"/>
       <c r="M52" s="83"/>
       <c r="N52" s="83"/>
       <c r="O52" s="83"/>
@@ -6604,52 +6598,52 @@
         <v>52</v>
       </c>
       <c r="C53" s="130"/>
-      <c r="D53" s="208" t="s">
+      <c r="D53" s="207" t="s">
         <v>63</v>
       </c>
-      <c r="E53" s="309">
+      <c r="E53" s="270">
         <f>SUM(E50:E52)</f>
         <v>0</v>
       </c>
-      <c r="F53" s="310">
+      <c r="F53" s="271">
         <f>SUM(F50:F52)</f>
         <v>0</v>
       </c>
-      <c r="G53" s="302">
+      <c r="G53" s="263">
         <f>SUM(G50:G52)</f>
         <v>0</v>
       </c>
-      <c r="H53" s="303"/>
+      <c r="H53" s="264"/>
       <c r="I53" s="132" t="s">
         <v>142</v>
       </c>
       <c r="J53" s="128"/>
-      <c r="L53" s="207"/>
+      <c r="L53" s="206"/>
     </row>
     <row r="54" spans="1:19" s="83" customFormat="1" ht="24" customHeight="1">
-      <c r="B54" s="209"/>
-      <c r="C54" s="209"/>
-      <c r="D54" s="210"/>
+      <c r="B54" s="208"/>
+      <c r="C54" s="208"/>
+      <c r="D54" s="209"/>
       <c r="E54" s="35"/>
       <c r="F54" s="36"/>
       <c r="G54" s="67"/>
       <c r="H54" s="143" t="s">
         <v>67</v>
       </c>
-      <c r="I54" s="211" t="s">
+      <c r="I54" s="210" t="s">
         <v>143</v>
       </c>
-      <c r="J54" s="212"/>
+      <c r="J54" s="211"/>
     </row>
     <row r="55" spans="1:19" s="83" customFormat="1" ht="24" customHeight="1">
       <c r="A55" s="138" t="s">
         <v>66</v>
       </c>
-      <c r="E55" s="213"/>
+      <c r="E55" s="212"/>
       <c r="I55" s="68" t="s">
         <v>144</v>
       </c>
-      <c r="J55" s="214"/>
+      <c r="J55" s="213"/>
       <c r="L55" s="98"/>
       <c r="M55" s="1"/>
       <c r="N55" s="1"/>
@@ -6732,10 +6726,10 @@
       <c r="S58" s="83"/>
     </row>
     <row r="59" spans="1:19" s="83" customFormat="1" ht="24.75" customHeight="1" thickTop="1">
-      <c r="A59" s="215" t="s">
+      <c r="A59" s="214" t="s">
         <v>31</v>
       </c>
-      <c r="B59" s="216" t="s">
+      <c r="B59" s="215" t="s">
         <v>99</v>
       </c>
       <c r="C59" s="171" t="s">
@@ -6748,12 +6742,12 @@
         <v>102</v>
       </c>
       <c r="F59" s="173"/>
-      <c r="G59" s="272" t="s">
+      <c r="G59" s="305" t="s">
         <v>103</v>
       </c>
-      <c r="H59" s="273"/>
-      <c r="I59" s="273"/>
-      <c r="J59" s="274"/>
+      <c r="H59" s="306"/>
+      <c r="I59" s="306"/>
+      <c r="J59" s="307"/>
       <c r="M59" s="6"/>
       <c r="N59" s="6"/>
       <c r="O59" s="6"/>
@@ -6762,7 +6756,7 @@
       <c r="R59" s="6"/>
     </row>
     <row r="60" spans="1:19" s="83" customFormat="1" ht="24.75" customHeight="1" thickBot="1">
-      <c r="A60" s="217" t="s">
+      <c r="A60" s="216" t="s">
         <v>40</v>
       </c>
       <c r="B60" s="119" t="s">
@@ -6771,17 +6765,17 @@
       <c r="C60" s="119" t="s">
         <v>106</v>
       </c>
-      <c r="D60" s="218" t="s">
+      <c r="D60" s="217" t="s">
         <v>107</v>
       </c>
       <c r="E60" s="181" t="s">
         <v>108</v>
       </c>
       <c r="F60" s="181"/>
-      <c r="G60" s="275"/>
-      <c r="H60" s="276"/>
-      <c r="I60" s="276"/>
-      <c r="J60" s="277"/>
+      <c r="G60" s="308"/>
+      <c r="H60" s="309"/>
+      <c r="I60" s="309"/>
+      <c r="J60" s="310"/>
       <c r="M60" s="6"/>
       <c r="N60" s="6"/>
       <c r="O60" s="6"/>
@@ -6790,21 +6784,21 @@
       <c r="R60" s="6"/>
     </row>
     <row r="61" spans="1:19" s="83" customFormat="1" ht="24.75" customHeight="1" thickTop="1">
-      <c r="A61" s="259" t="s">
+      <c r="A61" s="294" t="s">
         <v>146</v>
       </c>
       <c r="B61" s="126" t="s">
         <v>109</v>
       </c>
-      <c r="C61" s="219" t="s">
+      <c r="C61" s="218" t="s">
         <v>147</v>
       </c>
       <c r="D61" s="167"/>
-      <c r="E61" s="220" t="s">
+      <c r="E61" s="219" t="s">
         <v>148</v>
       </c>
-      <c r="F61" s="221"/>
-      <c r="G61" s="222" t="s">
+      <c r="F61" s="220"/>
+      <c r="G61" s="221" t="s">
         <v>112</v>
       </c>
       <c r="J61" s="137"/>
@@ -6816,24 +6810,24 @@
       <c r="R61" s="6"/>
     </row>
     <row r="62" spans="1:19" s="83" customFormat="1" ht="24.75" customHeight="1">
-      <c r="A62" s="260"/>
+      <c r="A62" s="295"/>
       <c r="B62" s="143" t="s">
         <v>116</v>
       </c>
-      <c r="C62" s="223" t="s">
+      <c r="C62" s="222" t="s">
         <v>149</v>
       </c>
       <c r="D62" s="143"/>
-      <c r="E62" s="224" t="s">
+      <c r="E62" s="223" t="s">
         <v>148</v>
       </c>
-      <c r="F62" s="224"/>
-      <c r="G62" s="213" t="s">
+      <c r="F62" s="223"/>
+      <c r="G62" s="212" t="s">
         <v>118</v>
       </c>
       <c r="H62" s="179"/>
       <c r="I62" s="179"/>
-      <c r="J62" s="225"/>
+      <c r="J62" s="224"/>
       <c r="M62" s="6"/>
       <c r="N62" s="6"/>
       <c r="O62" s="6"/>
@@ -6842,24 +6836,24 @@
       <c r="R62" s="6"/>
     </row>
     <row r="63" spans="1:19" s="83" customFormat="1" ht="24.75" customHeight="1" thickBot="1">
-      <c r="A63" s="261"/>
-      <c r="B63" s="226" t="s">
+      <c r="A63" s="296"/>
+      <c r="B63" s="225" t="s">
         <v>119</v>
       </c>
-      <c r="C63" s="227" t="s">
+      <c r="C63" s="226" t="s">
         <v>150</v>
       </c>
       <c r="D63" s="119"/>
-      <c r="E63" s="228" t="s">
+      <c r="E63" s="227" t="s">
         <v>148</v>
       </c>
-      <c r="F63" s="228"/>
+      <c r="F63" s="227"/>
       <c r="G63" s="104" t="s">
         <v>121</v>
       </c>
       <c r="H63" s="183"/>
       <c r="I63" s="183"/>
-      <c r="J63" s="229"/>
+      <c r="J63" s="228"/>
       <c r="M63" s="6"/>
       <c r="N63" s="6"/>
       <c r="O63" s="6"/>
@@ -6868,18 +6862,18 @@
       <c r="R63" s="6"/>
     </row>
     <row r="64" spans="1:19" s="83" customFormat="1" ht="27.6" thickTop="1" thickBot="1">
-      <c r="A64" s="230" t="s">
+      <c r="A64" s="229" t="s">
         <v>151</v>
       </c>
-      <c r="B64" s="231"/>
-      <c r="C64" s="231"/>
-      <c r="D64" s="231"/>
-      <c r="E64" s="231"/>
-      <c r="F64" s="231"/>
-      <c r="G64" s="231"/>
-      <c r="H64" s="231"/>
-      <c r="I64" s="231"/>
-      <c r="J64" s="232"/>
+      <c r="B64" s="230"/>
+      <c r="C64" s="230"/>
+      <c r="D64" s="230"/>
+      <c r="E64" s="230"/>
+      <c r="F64" s="230"/>
+      <c r="G64" s="230"/>
+      <c r="H64" s="230"/>
+      <c r="I64" s="230"/>
+      <c r="J64" s="231"/>
       <c r="M64" s="6"/>
       <c r="N64" s="6"/>
       <c r="O64" s="6"/>
@@ -6888,7 +6882,7 @@
       <c r="R64" s="6"/>
     </row>
     <row r="65" spans="1:18" s="83" customFormat="1" ht="21" thickTop="1">
-      <c r="A65" s="233"/>
+      <c r="A65" s="232"/>
       <c r="J65" s="137"/>
       <c r="M65" s="6"/>
       <c r="N65" s="6"/>
@@ -6898,16 +6892,16 @@
       <c r="R65" s="6"/>
     </row>
     <row r="66" spans="1:18" s="83" customFormat="1" ht="20.399999999999999">
-      <c r="A66" s="234"/>
-      <c r="B66" s="235"/>
-      <c r="C66" s="235"/>
-      <c r="D66" s="235"/>
-      <c r="E66" s="235"/>
-      <c r="F66" s="235"/>
-      <c r="G66" s="235"/>
-      <c r="H66" s="235"/>
-      <c r="I66" s="235"/>
-      <c r="J66" s="236"/>
+      <c r="A66" s="233"/>
+      <c r="B66" s="234"/>
+      <c r="C66" s="234"/>
+      <c r="D66" s="234"/>
+      <c r="E66" s="234"/>
+      <c r="F66" s="234"/>
+      <c r="G66" s="234"/>
+      <c r="H66" s="234"/>
+      <c r="I66" s="234"/>
+      <c r="J66" s="235"/>
       <c r="M66" s="6"/>
       <c r="N66" s="6"/>
       <c r="O66" s="6"/>
@@ -6916,16 +6910,16 @@
       <c r="R66" s="6"/>
     </row>
     <row r="67" spans="1:18" s="83" customFormat="1" ht="20.399999999999999">
-      <c r="A67" s="234"/>
-      <c r="B67" s="235"/>
-      <c r="C67" s="235"/>
-      <c r="D67" s="235"/>
-      <c r="E67" s="235"/>
-      <c r="F67" s="235"/>
-      <c r="G67" s="235"/>
-      <c r="H67" s="235"/>
-      <c r="I67" s="235"/>
-      <c r="J67" s="236"/>
+      <c r="A67" s="233"/>
+      <c r="B67" s="234"/>
+      <c r="C67" s="234"/>
+      <c r="D67" s="234"/>
+      <c r="E67" s="234"/>
+      <c r="F67" s="234"/>
+      <c r="G67" s="234"/>
+      <c r="H67" s="234"/>
+      <c r="I67" s="234"/>
+      <c r="J67" s="235"/>
       <c r="M67" s="6"/>
       <c r="N67" s="6"/>
       <c r="O67" s="6"/>
@@ -6934,16 +6928,16 @@
       <c r="R67" s="6"/>
     </row>
     <row r="68" spans="1:18" s="83" customFormat="1" ht="20.399999999999999">
-      <c r="A68" s="234"/>
-      <c r="B68" s="235"/>
-      <c r="C68" s="235"/>
-      <c r="D68" s="235"/>
-      <c r="E68" s="235"/>
-      <c r="F68" s="235"/>
-      <c r="G68" s="235"/>
-      <c r="H68" s="235"/>
-      <c r="I68" s="235"/>
-      <c r="J68" s="236"/>
+      <c r="A68" s="233"/>
+      <c r="B68" s="234"/>
+      <c r="C68" s="234"/>
+      <c r="D68" s="234"/>
+      <c r="E68" s="234"/>
+      <c r="F68" s="234"/>
+      <c r="G68" s="234"/>
+      <c r="H68" s="234"/>
+      <c r="I68" s="234"/>
+      <c r="J68" s="235"/>
       <c r="M68" s="6"/>
       <c r="N68" s="6"/>
       <c r="O68" s="6"/>
@@ -6952,16 +6946,16 @@
       <c r="R68" s="6"/>
     </row>
     <row r="69" spans="1:18" s="83" customFormat="1" ht="20.399999999999999">
-      <c r="A69" s="234"/>
-      <c r="B69" s="235"/>
-      <c r="C69" s="235"/>
-      <c r="D69" s="235"/>
-      <c r="E69" s="235"/>
-      <c r="F69" s="235"/>
-      <c r="G69" s="235"/>
-      <c r="H69" s="235"/>
-      <c r="I69" s="235"/>
-      <c r="J69" s="236"/>
+      <c r="A69" s="233"/>
+      <c r="B69" s="234"/>
+      <c r="C69" s="234"/>
+      <c r="D69" s="234"/>
+      <c r="E69" s="234"/>
+      <c r="F69" s="234"/>
+      <c r="G69" s="234"/>
+      <c r="H69" s="234"/>
+      <c r="I69" s="234"/>
+      <c r="J69" s="235"/>
       <c r="M69" s="6"/>
       <c r="N69" s="6"/>
       <c r="O69" s="6"/>
@@ -6970,16 +6964,16 @@
       <c r="R69" s="6"/>
     </row>
     <row r="70" spans="1:18" s="83" customFormat="1" ht="20.399999999999999">
-      <c r="A70" s="234"/>
-      <c r="B70" s="235"/>
-      <c r="C70" s="235"/>
-      <c r="D70" s="235"/>
-      <c r="E70" s="235"/>
-      <c r="F70" s="235"/>
-      <c r="G70" s="235"/>
-      <c r="H70" s="235"/>
-      <c r="I70" s="235"/>
-      <c r="J70" s="236"/>
+      <c r="A70" s="233"/>
+      <c r="B70" s="234"/>
+      <c r="C70" s="234"/>
+      <c r="D70" s="234"/>
+      <c r="E70" s="234"/>
+      <c r="F70" s="234"/>
+      <c r="G70" s="234"/>
+      <c r="H70" s="234"/>
+      <c r="I70" s="234"/>
+      <c r="J70" s="235"/>
       <c r="M70" s="6"/>
       <c r="N70" s="6"/>
       <c r="O70" s="6"/>
@@ -6988,16 +6982,16 @@
       <c r="R70" s="6"/>
     </row>
     <row r="71" spans="1:18" s="83" customFormat="1" ht="20.399999999999999">
-      <c r="A71" s="234"/>
-      <c r="B71" s="235"/>
-      <c r="C71" s="235"/>
-      <c r="D71" s="235"/>
-      <c r="E71" s="235"/>
-      <c r="F71" s="235"/>
-      <c r="G71" s="235"/>
-      <c r="H71" s="235"/>
-      <c r="I71" s="235"/>
-      <c r="J71" s="236"/>
+      <c r="A71" s="233"/>
+      <c r="B71" s="234"/>
+      <c r="C71" s="234"/>
+      <c r="D71" s="234"/>
+      <c r="E71" s="234"/>
+      <c r="F71" s="234"/>
+      <c r="G71" s="234"/>
+      <c r="H71" s="234"/>
+      <c r="I71" s="234"/>
+      <c r="J71" s="235"/>
       <c r="M71" s="6"/>
       <c r="N71" s="6"/>
       <c r="O71" s="6"/>
@@ -7006,16 +7000,16 @@
       <c r="R71" s="6"/>
     </row>
     <row r="72" spans="1:18" s="83" customFormat="1" ht="20.399999999999999">
-      <c r="A72" s="234"/>
-      <c r="B72" s="235"/>
-      <c r="C72" s="235"/>
-      <c r="D72" s="235"/>
-      <c r="E72" s="235"/>
-      <c r="F72" s="235"/>
-      <c r="G72" s="235"/>
-      <c r="H72" s="235"/>
-      <c r="I72" s="235"/>
-      <c r="J72" s="236"/>
+      <c r="A72" s="233"/>
+      <c r="B72" s="234"/>
+      <c r="C72" s="234"/>
+      <c r="D72" s="234"/>
+      <c r="E72" s="234"/>
+      <c r="F72" s="234"/>
+      <c r="G72" s="234"/>
+      <c r="H72" s="234"/>
+      <c r="I72" s="234"/>
+      <c r="J72" s="235"/>
       <c r="M72" s="6"/>
       <c r="N72" s="6"/>
       <c r="O72" s="6"/>
@@ -7024,16 +7018,16 @@
       <c r="R72" s="6"/>
     </row>
     <row r="73" spans="1:18" s="83" customFormat="1" ht="20.399999999999999">
-      <c r="A73" s="234"/>
-      <c r="B73" s="235"/>
-      <c r="C73" s="235"/>
-      <c r="D73" s="235"/>
-      <c r="E73" s="235"/>
-      <c r="F73" s="235"/>
-      <c r="G73" s="235"/>
-      <c r="H73" s="235"/>
-      <c r="I73" s="235"/>
-      <c r="J73" s="236"/>
+      <c r="A73" s="233"/>
+      <c r="B73" s="234"/>
+      <c r="C73" s="234"/>
+      <c r="D73" s="234"/>
+      <c r="E73" s="234"/>
+      <c r="F73" s="234"/>
+      <c r="G73" s="234"/>
+      <c r="H73" s="234"/>
+      <c r="I73" s="234"/>
+      <c r="J73" s="235"/>
       <c r="M73" s="6"/>
       <c r="N73" s="6"/>
       <c r="O73" s="6"/>
@@ -7042,16 +7036,16 @@
       <c r="R73" s="6"/>
     </row>
     <row r="74" spans="1:18" s="83" customFormat="1" ht="20.399999999999999">
-      <c r="A74" s="234"/>
-      <c r="B74" s="235"/>
-      <c r="C74" s="235"/>
-      <c r="D74" s="235"/>
-      <c r="E74" s="235"/>
-      <c r="F74" s="235"/>
-      <c r="G74" s="235"/>
-      <c r="H74" s="235"/>
-      <c r="I74" s="235"/>
-      <c r="J74" s="236"/>
+      <c r="A74" s="233"/>
+      <c r="B74" s="234"/>
+      <c r="C74" s="234"/>
+      <c r="D74" s="234"/>
+      <c r="E74" s="234"/>
+      <c r="F74" s="234"/>
+      <c r="G74" s="234"/>
+      <c r="H74" s="234"/>
+      <c r="I74" s="234"/>
+      <c r="J74" s="235"/>
       <c r="M74" s="6"/>
       <c r="N74" s="6"/>
       <c r="O74" s="6"/>
@@ -7060,16 +7054,16 @@
       <c r="R74" s="6"/>
     </row>
     <row r="75" spans="1:18" s="83" customFormat="1" ht="20.399999999999999">
-      <c r="A75" s="234"/>
-      <c r="B75" s="235"/>
-      <c r="C75" s="235"/>
-      <c r="D75" s="235"/>
-      <c r="E75" s="235"/>
-      <c r="F75" s="235"/>
-      <c r="G75" s="235"/>
-      <c r="H75" s="235"/>
-      <c r="I75" s="235"/>
-      <c r="J75" s="236"/>
+      <c r="A75" s="233"/>
+      <c r="B75" s="234"/>
+      <c r="C75" s="234"/>
+      <c r="D75" s="234"/>
+      <c r="E75" s="234"/>
+      <c r="F75" s="234"/>
+      <c r="G75" s="234"/>
+      <c r="H75" s="234"/>
+      <c r="I75" s="234"/>
+      <c r="J75" s="235"/>
       <c r="M75" s="6"/>
       <c r="N75" s="6"/>
       <c r="O75" s="6"/>
@@ -7078,16 +7072,16 @@
       <c r="R75" s="6"/>
     </row>
     <row r="76" spans="1:18" s="83" customFormat="1" ht="20.399999999999999">
-      <c r="A76" s="234"/>
-      <c r="B76" s="235"/>
-      <c r="C76" s="235"/>
-      <c r="D76" s="235"/>
-      <c r="E76" s="235"/>
-      <c r="F76" s="235"/>
-      <c r="G76" s="235"/>
-      <c r="H76" s="235"/>
-      <c r="I76" s="235"/>
-      <c r="J76" s="236"/>
+      <c r="A76" s="233"/>
+      <c r="B76" s="234"/>
+      <c r="C76" s="234"/>
+      <c r="D76" s="234"/>
+      <c r="E76" s="234"/>
+      <c r="F76" s="234"/>
+      <c r="G76" s="234"/>
+      <c r="H76" s="234"/>
+      <c r="I76" s="234"/>
+      <c r="J76" s="235"/>
       <c r="M76" s="6"/>
       <c r="N76" s="6"/>
       <c r="O76" s="6"/>
@@ -7096,16 +7090,16 @@
       <c r="R76" s="6"/>
     </row>
     <row r="77" spans="1:18" s="83" customFormat="1" ht="20.399999999999999">
-      <c r="A77" s="234"/>
-      <c r="B77" s="235"/>
-      <c r="C77" s="235"/>
-      <c r="D77" s="235"/>
-      <c r="E77" s="235"/>
-      <c r="F77" s="235"/>
-      <c r="G77" s="235"/>
-      <c r="H77" s="235"/>
-      <c r="I77" s="235"/>
-      <c r="J77" s="236"/>
+      <c r="A77" s="233"/>
+      <c r="B77" s="234"/>
+      <c r="C77" s="234"/>
+      <c r="D77" s="234"/>
+      <c r="E77" s="234"/>
+      <c r="F77" s="234"/>
+      <c r="G77" s="234"/>
+      <c r="H77" s="234"/>
+      <c r="I77" s="234"/>
+      <c r="J77" s="235"/>
       <c r="M77" s="6"/>
       <c r="N77" s="6"/>
       <c r="O77" s="6"/>
@@ -7114,16 +7108,16 @@
       <c r="R77" s="6"/>
     </row>
     <row r="78" spans="1:18" s="83" customFormat="1" ht="20.399999999999999">
-      <c r="A78" s="234"/>
-      <c r="B78" s="235"/>
-      <c r="C78" s="235"/>
-      <c r="D78" s="235"/>
-      <c r="E78" s="235"/>
-      <c r="F78" s="235"/>
-      <c r="G78" s="235"/>
-      <c r="H78" s="235"/>
-      <c r="I78" s="235"/>
-      <c r="J78" s="236"/>
+      <c r="A78" s="233"/>
+      <c r="B78" s="234"/>
+      <c r="C78" s="234"/>
+      <c r="D78" s="234"/>
+      <c r="E78" s="234"/>
+      <c r="F78" s="234"/>
+      <c r="G78" s="234"/>
+      <c r="H78" s="234"/>
+      <c r="I78" s="234"/>
+      <c r="J78" s="235"/>
       <c r="M78" s="6"/>
       <c r="N78" s="6"/>
       <c r="O78" s="6"/>
@@ -7132,7 +7126,7 @@
       <c r="R78" s="6"/>
     </row>
     <row r="79" spans="1:18" s="83" customFormat="1" ht="21" thickBot="1">
-      <c r="A79" s="237"/>
+      <c r="A79" s="236"/>
       <c r="B79" s="183"/>
       <c r="C79" s="183"/>
       <c r="D79" s="183"/>
@@ -7141,7 +7135,7 @@
       <c r="G79" s="183"/>
       <c r="H79" s="183"/>
       <c r="I79" s="183"/>
-      <c r="J79" s="229"/>
+      <c r="J79" s="228"/>
       <c r="M79" s="6"/>
       <c r="N79" s="6"/>
       <c r="O79" s="6"/>
@@ -7150,11 +7144,11 @@
       <c r="R79" s="6"/>
     </row>
     <row r="80" spans="1:18" s="83" customFormat="1" ht="21" thickTop="1">
-      <c r="A80" s="262" t="s">
+      <c r="A80" s="297" t="s">
         <v>129</v>
       </c>
-      <c r="B80" s="263"/>
-      <c r="C80" s="263"/>
+      <c r="B80" s="298"/>
+      <c r="C80" s="298"/>
       <c r="D80" s="184"/>
       <c r="E80" s="185" t="s">
         <v>130</v>
@@ -7176,9 +7170,9 @@
       <c r="R80" s="6"/>
     </row>
     <row r="81" spans="1:19" s="83" customFormat="1" ht="21" thickBot="1">
-      <c r="A81" s="264"/>
-      <c r="B81" s="265"/>
-      <c r="C81" s="265"/>
+      <c r="A81" s="299"/>
+      <c r="B81" s="300"/>
+      <c r="C81" s="300"/>
       <c r="D81" s="189"/>
       <c r="E81" s="190" t="s">
         <v>133</v>
@@ -7192,14 +7186,14 @@
         <v>132</v>
       </c>
       <c r="J81" s="193"/>
-      <c r="L81" s="238"/>
+      <c r="L81" s="237"/>
       <c r="M81" s="6"/>
       <c r="N81" s="6"/>
       <c r="O81" s="6"/>
       <c r="P81" s="6"/>
       <c r="Q81" s="6"/>
       <c r="R81" s="6"/>
-      <c r="S81" s="238"/>
+      <c r="S81" s="237"/>
     </row>
     <row r="82" spans="1:19" s="83" customFormat="1" ht="21" thickBot="1">
       <c r="A82" s="194" t="s">
@@ -7212,38 +7206,25 @@
       <c r="F82" s="195"/>
       <c r="G82" s="195"/>
       <c r="H82" s="195"/>
-      <c r="I82" s="266" t="s">
+      <c r="I82" s="301" t="s">
         <v>136</v>
       </c>
-      <c r="J82" s="267"/>
-      <c r="L82" s="238"/>
+      <c r="J82" s="302"/>
+      <c r="L82" s="237"/>
       <c r="M82" s="6"/>
       <c r="N82" s="6"/>
       <c r="O82" s="6"/>
       <c r="P82" s="6"/>
       <c r="Q82" s="6"/>
       <c r="R82" s="6"/>
-      <c r="S82" s="238"/>
+      <c r="S82" s="237"/>
     </row>
   </sheetData>
   <protectedRanges>
     <protectedRange sqref="B4" name="Range2_1"/>
     <protectedRange sqref="G4" name="Range1_1"/>
   </protectedRanges>
-  <mergeCells count="22">
-    <mergeCell ref="G30:J31"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="I3:J4"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="I34:J34"/>
-    <mergeCell ref="A35:A37"/>
-    <mergeCell ref="I35:J35"/>
-    <mergeCell ref="I36:J36"/>
-    <mergeCell ref="I37:J37"/>
+  <mergeCells count="23">
     <mergeCell ref="A61:A63"/>
     <mergeCell ref="A80:C81"/>
     <mergeCell ref="I82:J82"/>
@@ -7253,6 +7234,20 @@
     <mergeCell ref="I43:J43"/>
     <mergeCell ref="I44:J45"/>
     <mergeCell ref="G59:J60"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="I34:J34"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="I35:J35"/>
+    <mergeCell ref="I36:J36"/>
+    <mergeCell ref="I37:J37"/>
+    <mergeCell ref="G30:J31"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="I3:J4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>